<commit_message>
plano de ação sprint 2B
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/2°Semestre/PI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/2°Semestre/PI/Noctoramento/Documentacao/Documentação do Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{8C25980D-4FEE-4CE7-A332-8BA0992E413C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{575F727D-9020-42BD-AB8C-5177186A0AF0}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{8C25980D-4FEE-4CE7-A332-8BA0992E413C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62362B63-F7DA-4B13-BA40-CD9B095EC472}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -213,6 +213,27 @@
   </si>
   <si>
     <t xml:space="preserve">    Yuri</t>
+  </si>
+  <si>
+    <t>BPMN</t>
+  </si>
+  <si>
+    <t>DER</t>
+  </si>
+  <si>
+    <t>JAR conectado ao BD</t>
+  </si>
+  <si>
+    <t>JAR rodando em cliente linux</t>
+  </si>
+  <si>
+    <t>JAR listando processos Disco...</t>
+  </si>
+  <si>
+    <t>Protótivo funcional do java (interoperabilidade)</t>
+  </si>
+  <si>
+    <t>JAR listando informações do hardware</t>
   </si>
 </sst>
 </file>
@@ -614,6 +635,9 @@
     <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -637,9 +661,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1020,8 +1041,8 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1038,24 +1059,24 @@
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:16" s="6" customFormat="1" ht="22.2" customHeight="1">
       <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="44"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="38"/>
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
@@ -1073,14 +1094,14 @@
       <c r="B3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="51"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1246,7 +1267,7 @@
       <c r="B12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="43" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="11"/>
@@ -1311,18 +1332,24 @@
       <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:16" ht="39" customHeight="1">
-      <c r="B16" s="11"/>
+      <c r="B16" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="36">
-        <v>0.25</v>
-      </c>
-      <c r="F16" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="19">
+        <v>45390</v>
+      </c>
       <c r="G16" s="19"/>
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="67.2" customHeight="1">
-      <c r="B17" s="11"/>
+      <c r="B17" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
         <v>21</v>
@@ -1330,25 +1357,33 @@
       <c r="E17" s="36">
         <v>0</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="19">
+        <v>45390</v>
+      </c>
       <c r="G17" s="19"/>
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="2:8" ht="49.2" customHeight="1">
-      <c r="B18" s="11"/>
+      <c r="B18" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="36">
-        <v>0</v>
-      </c>
-      <c r="F18" s="19"/>
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="19">
+        <v>45390</v>
+      </c>
       <c r="G18" s="19"/>
       <c r="H18" s="18"/>
     </row>
     <row r="19" spans="2:8" ht="45.6" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
         <v>21</v>
@@ -1356,12 +1391,16 @@
       <c r="E19" s="36">
         <v>0</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="19">
+        <v>45390</v>
+      </c>
       <c r="G19" s="19"/>
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="2:8" ht="49.8" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
         <v>21</v>
@@ -1369,12 +1408,16 @@
       <c r="E20" s="36">
         <v>0</v>
       </c>
-      <c r="F20" s="19"/>
+      <c r="F20" s="19">
+        <v>45390</v>
+      </c>
       <c r="G20" s="19"/>
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="2:8" ht="19.95" customHeight="1">
-      <c r="B21" s="11"/>
+      <c r="B21" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
         <v>21</v>
@@ -1382,25 +1425,35 @@
       <c r="E21" s="36">
         <v>0</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="19">
+        <v>45390</v>
+      </c>
       <c r="G21" s="19"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="2:8" ht="19.95" customHeight="1">
-      <c r="B22" s="18"/>
+    <row r="22" spans="2:8">
+      <c r="B22" s="18" t="s">
+        <v>59</v>
+      </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="19"/>
+      <c r="F22" s="19">
+        <v>45390</v>
+      </c>
       <c r="G22" s="19"/>
       <c r="H22" s="18"/>
     </row>
     <row r="23" spans="2:8" ht="19.95" customHeight="1">
-      <c r="B23" s="18"/>
+      <c r="B23" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
-      <c r="F23" s="19"/>
+      <c r="F23" s="19">
+        <v>45390</v>
+      </c>
       <c r="G23" s="19"/>
       <c r="H23" s="18"/>
     </row>
@@ -1758,7 +1811,7 @@
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="83" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="83" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Atualização Plano de ação
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/2°Semestre/PI/Noctoramento/Documentacao/Documentação do Projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sp-tech\NocToramento\Documentacao\Documentação do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{8C25980D-4FEE-4CE7-A332-8BA0992E413C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62362B63-F7DA-4B13-BA40-CD9B095EC472}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA92C73-644D-428C-9C51-4F89D6D00EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Ação" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plano de Ação'!$B$1:$H$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plano de Ação'!$B$1:$H$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Plano de Ação - EM BRANCO'!$B$1:$H$28</definedName>
     <definedName name="Interval" localSheetId="1">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="Interval">'[1]Return to Work Template'!#REF!</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -206,9 +206,6 @@
     <t xml:space="preserve">Pedro Sarabando e Nathalia  </t>
   </si>
   <si>
-    <t xml:space="preserve">Luis </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Yuri</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>BPMN</t>
   </si>
   <si>
-    <t>DER</t>
-  </si>
-  <si>
     <t>JAR conectado ao BD</t>
   </si>
   <si>
@@ -234,6 +228,44 @@
   </si>
   <si>
     <t>JAR listando informações do hardware</t>
+  </si>
+  <si>
+    <t>Luiz Fernando</t>
+  </si>
+  <si>
+    <t>Espicifação Funcional de (3) Itens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro Souza
+Pedro Sarabando </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cruds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deixar telas cadastro e login respansivas </t>
+  </si>
+  <si>
+    <t>Tela cadatrar funcionario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+tela cadatrar maquina </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tela Redefinir senha </t>
+  </si>
+  <si>
+    <t>Desejavel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualizar DER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuri </t>
+  </si>
+  <si>
+    <t>Atualizar users stories e proto persona</t>
   </si>
 </sst>
 </file>
@@ -1038,23 +1070,23 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="3.296875" customWidth="1"/>
-    <col min="2" max="2" width="44.59765625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="44.58203125" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.69921875" customWidth="1"/>
-    <col min="6" max="6" width="17.59765625" customWidth="1"/>
-    <col min="7" max="7" width="12.296875" customWidth="1"/>
-    <col min="8" max="8" width="42.19921875" customWidth="1"/>
-    <col min="9" max="9" width="3.296875" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.58203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="42.1640625" customWidth="1"/>
+    <col min="9" max="9" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
@@ -1069,7 +1101,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" ht="22.2" customHeight="1">
+    <row r="2" spans="1:16" s="6" customFormat="1" ht="22.25" customHeight="1">
       <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
@@ -1090,7 +1122,7 @@
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
     </row>
-    <row r="3" spans="1:16" s="6" customFormat="1" ht="22.2" customHeight="1">
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="22.25" customHeight="1">
       <c r="B3" s="28" t="s">
         <v>44</v>
       </c>
@@ -1111,7 +1143,7 @@
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" spans="1:16" ht="10.95" customHeight="1">
+    <row r="4" spans="1:16" ht="11" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1120,7 +1152,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:16" ht="19.95" customHeight="1">
+    <row r="5" spans="1:16" ht="20" customHeight="1">
       <c r="B5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1143,7 +1175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="19.95" customHeight="1">
+    <row r="6" spans="1:16" ht="20" customHeight="1">
       <c r="B6" s="21" t="s">
         <v>16</v>
       </c>
@@ -1154,7 +1186,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="52.2" customHeight="1">
+    <row r="7" spans="1:16" ht="52.25" customHeight="1">
       <c r="B7" s="11" t="s">
         <v>48</v>
       </c>
@@ -1165,7 +1197,7 @@
         <v>21</v>
       </c>
       <c r="E7" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F7" s="37">
         <v>45380</v>
@@ -1177,18 +1209,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="39.6" customHeight="1">
+    <row r="8" spans="1:16" ht="39.65" customHeight="1">
       <c r="B8" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="36">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F8" s="37">
         <v>45381</v>
@@ -1209,7 +1241,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="36">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="F9" s="37">
         <v>45381</v>
@@ -1219,16 +1251,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="70.2" customHeight="1">
+    <row r="10" spans="1:16" ht="70.25" customHeight="1">
       <c r="B10" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="E10" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="37">
         <v>45381</v>
@@ -1245,7 +1279,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>21</v>
@@ -1263,15 +1297,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="19.95" customHeight="1">
+    <row r="12" spans="1:16" ht="20" customHeight="1">
       <c r="B12" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="36">
+        <v>0.5</v>
+      </c>
       <c r="F12" s="19">
         <v>45381</v>
       </c>
@@ -1280,15 +1318,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="19.95" customHeight="1">
+    <row r="13" spans="1:16" ht="20" customHeight="1">
       <c r="B13" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+        <v>59</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="36">
+        <v>0.9</v>
+      </c>
       <c r="F13" s="19">
         <v>45381</v>
       </c>
@@ -1297,7 +1339,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="19.95" customHeight="1">
+    <row r="14" spans="1:16" ht="20" customHeight="1">
       <c r="B14" s="40" t="s">
         <v>3</v>
       </c>
@@ -1320,7 +1362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="19.95" customHeight="1">
+    <row r="15" spans="1:16" ht="20" customHeight="1">
       <c r="B15" s="21" t="s">
         <v>19</v>
       </c>
@@ -1335,10 +1377,14 @@
       <c r="B16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="E16" s="36">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F16" s="19">
         <v>45390</v>
@@ -1346,13 +1392,13 @@
       <c r="G16" s="19"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="2:8" ht="67.2" customHeight="1">
+    <row r="17" spans="2:8" ht="39" customHeight="1">
       <c r="B17" s="11" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="E17" s="36">
         <v>0</v>
@@ -1361,30 +1407,34 @@
         <v>45390</v>
       </c>
       <c r="G17" s="19"/>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" spans="2:8" ht="49.2" customHeight="1">
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="2:8" ht="39" customHeight="1">
       <c r="B18" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="11"/>
+        <v>64</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="D18" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="36">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F18" s="19">
         <v>45390</v>
       </c>
       <c r="G18" s="19"/>
-      <c r="H18" s="18"/>
-    </row>
-    <row r="19" spans="2:8" ht="45.6" customHeight="1">
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="2:8" ht="39.5" customHeight="1">
       <c r="B19" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="11"/>
+        <v>65</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="D19" s="11" t="s">
         <v>21</v>
       </c>
@@ -1395,13 +1445,15 @@
         <v>45390</v>
       </c>
       <c r="G19" s="19"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="2:8" ht="49.8" customHeight="1">
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="2:8" ht="39.5" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="D20" s="11" t="s">
         <v>21</v>
       </c>
@@ -1412,11 +1464,11 @@
         <v>45390</v>
       </c>
       <c r="G20" s="19"/>
-      <c r="H20" s="18"/>
-    </row>
-    <row r="21" spans="2:8" ht="19.95" customHeight="1">
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="2:8" ht="39" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
@@ -1429,378 +1481,502 @@
         <v>45390</v>
       </c>
       <c r="G21" s="19"/>
-      <c r="H21" s="18"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="2:8" ht="39" customHeight="1">
+      <c r="B22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="36">
+        <v>0</v>
+      </c>
       <c r="F22" s="19">
         <v>45390</v>
       </c>
       <c r="G22" s="19"/>
-      <c r="H22" s="18"/>
-    </row>
-    <row r="23" spans="2:8" ht="19.95" customHeight="1">
-      <c r="B23" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="2:8" ht="67.25" customHeight="1">
+      <c r="B23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="36">
+        <v>0</v>
+      </c>
       <c r="F23" s="19">
         <v>45390</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="18"/>
     </row>
-    <row r="24" spans="2:8" ht="19.95" customHeight="1">
-      <c r="B24" s="18"/>
+    <row r="24" spans="2:8" ht="49.25" customHeight="1">
+      <c r="B24" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="D24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="19">
+        <v>45390</v>
+      </c>
+      <c r="G24" s="19"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="2:8" ht="27" customHeight="1">
-      <c r="B25" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="B26" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" spans="2:8" ht="28.2" customHeight="1">
-      <c r="B27" s="11"/>
+    <row r="25" spans="2:8" ht="45.65" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="36">
+        <v>0</v>
+      </c>
+      <c r="F25" s="19">
+        <v>45390</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="2:8" ht="49.75" customHeight="1">
+      <c r="B26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="36">
+        <v>0</v>
+      </c>
+      <c r="F26" s="19">
+        <v>45390</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B27" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="F27" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="19">
+        <v>45390</v>
+      </c>
       <c r="G27" s="19"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="26.4" customHeight="1">
-      <c r="B28" s="11"/>
+    <row r="28" spans="2:8" ht="36.5" customHeight="1">
+      <c r="B28" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="36">
-        <v>0.75</v>
-      </c>
-      <c r="F28" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="19">
+        <v>45390</v>
+      </c>
       <c r="G28" s="19"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="2:8" ht="21" customHeight="1">
-      <c r="B29" s="11"/>
+    <row r="29" spans="2:8" ht="28.5" customHeight="1">
+      <c r="B29" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E29" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="F29" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="19">
+        <v>45390</v>
+      </c>
       <c r="G29" s="19"/>
       <c r="H29" s="18"/>
     </row>
-    <row r="30" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
+    <row r="30" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B30" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="D30" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E30" s="36">
-        <v>0.6</v>
-      </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="19">
+        <v>45390</v>
+      </c>
+      <c r="G30" s="12"/>
       <c r="H30" s="18"/>
     </row>
     <row r="31" spans="2:8" ht="27" customHeight="1">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="36">
-        <v>0</v>
-      </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="18"/>
-    </row>
-    <row r="32" spans="2:8" ht="28.2" customHeight="1">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="36">
-        <v>0</v>
-      </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="11"/>
-    </row>
-    <row r="33" spans="2:8" ht="24" customHeight="1">
-      <c r="B33" s="18"/>
+      <c r="B31" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" s="1" customFormat="1" ht="24" customHeight="1">
+      <c r="B32" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" spans="2:8" ht="28.25" customHeight="1">
+      <c r="B33" s="11"/>
       <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="D33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="36">
+        <v>0.5</v>
+      </c>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
       <c r="H33" s="18"/>
     </row>
-    <row r="34" spans="2:8" ht="27.6" customHeight="1">
-      <c r="B34" s="18"/>
+    <row r="34" spans="2:8" ht="26.4" customHeight="1">
+      <c r="B34" s="11"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
+      <c r="D34" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="36">
+        <v>0.75</v>
+      </c>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
       <c r="H34" s="18"/>
     </row>
-    <row r="35" spans="2:8" ht="25.2" customHeight="1">
-      <c r="B35" s="18"/>
+    <row r="35" spans="2:8" ht="21" customHeight="1">
+      <c r="B35" s="11"/>
       <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
+      <c r="D35" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="36">
+        <v>0.8</v>
+      </c>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="2:8" ht="24" customHeight="1">
-      <c r="B36" s="18"/>
+    <row r="36" spans="2:8" ht="23.4" customHeight="1">
+      <c r="B36" s="11"/>
       <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+      <c r="D36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="36">
+        <v>0.6</v>
+      </c>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="23" t="s">
+    <row r="37" spans="2:8" ht="27" customHeight="1">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="36">
+        <v>0</v>
+      </c>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="2:8" ht="28.25" customHeight="1">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="36">
+        <v>0</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="2:8" ht="24" customHeight="1">
+      <c r="B39" s="18"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="18"/>
+    </row>
+    <row r="40" spans="2:8" ht="27.65" customHeight="1">
+      <c r="B40" s="18"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="2:8" ht="25.25" customHeight="1">
+      <c r="B41" s="18"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="2:8" ht="24" customHeight="1">
+      <c r="B42" s="18"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="23"/>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="21"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="21"/>
-    </row>
-    <row r="39" spans="2:8" ht="25.8" customHeight="1">
-      <c r="B39" s="26"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="26"/>
-    </row>
-    <row r="40" spans="2:8" ht="39" customHeight="1">
-      <c r="B40" s="26" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="23"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="21"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="21"/>
+    </row>
+    <row r="45" spans="2:8" ht="25.75" customHeight="1">
+      <c r="B45" s="26"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="26"/>
+    </row>
+    <row r="46" spans="2:8" ht="39" customHeight="1">
+      <c r="B46" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C46" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="42">
+      <c r="D46" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="42">
         <v>0.3</v>
       </c>
-      <c r="F40" s="32">
+      <c r="F46" s="32">
         <v>45219</v>
       </c>
-      <c r="G40" s="32">
+      <c r="G46" s="32">
         <v>45222</v>
       </c>
-      <c r="H40" s="26" t="s">
+      <c r="H46" s="26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="33" customHeight="1">
-      <c r="B41" s="26" t="s">
+    <row r="47" spans="2:8" ht="33" customHeight="1">
+      <c r="B47" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C47" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" s="42">
+      <c r="D47" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="42">
         <v>0.4</v>
       </c>
-      <c r="F41" s="32">
+      <c r="F47" s="32">
         <v>45219</v>
       </c>
-      <c r="G41" s="32">
+      <c r="G47" s="32">
         <v>45222</v>
       </c>
-      <c r="H41" s="26" t="s">
+      <c r="H47" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="36.6" customHeight="1">
-      <c r="B42" s="18" t="s">
+    <row r="48" spans="2:8" ht="36.65" customHeight="1">
+      <c r="B48" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C48" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="36">
+      <c r="D48" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="36">
         <v>0</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F48" s="19">
         <v>45219</v>
       </c>
-      <c r="G42" s="19">
+      <c r="G48" s="19">
         <v>45222</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H48" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="34.799999999999997" customHeight="1">
-      <c r="B43" s="26"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="26"/>
-    </row>
-    <row r="44" spans="2:8" ht="37.799999999999997" customHeight="1">
-      <c r="B44" s="26"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="26"/>
-    </row>
-    <row r="45" spans="2:8" ht="34.200000000000003" customHeight="1">
-      <c r="B45" s="18"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="18"/>
-    </row>
-    <row r="46" spans="2:8" ht="37.799999999999997" customHeight="1">
-      <c r="B46" s="26"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="26"/>
-    </row>
-    <row r="47" spans="2:8" ht="37.200000000000003" customHeight="1">
-      <c r="B47" s="26"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="26"/>
-    </row>
-    <row r="48" spans="2:8" ht="37.200000000000003" customHeight="1">
-      <c r="B48" s="18"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="18"/>
-    </row>
-    <row r="49" spans="2:8">
-      <c r="B49" s="33"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="33"/>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" s="33"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="33"/>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" s="33"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="33"/>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+    <row r="49" spans="2:8" ht="34.75" customHeight="1">
+      <c r="B49" s="26"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="26"/>
+    </row>
+    <row r="50" spans="2:8" ht="37.75" customHeight="1">
+      <c r="B50" s="26"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="26"/>
+    </row>
+    <row r="51" spans="2:8" ht="34.25" customHeight="1">
+      <c r="B51" s="18"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="2:8" ht="37.75" customHeight="1">
+      <c r="B52" s="26"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="26"/>
+    </row>
+    <row r="53" spans="2:8" ht="37.25" customHeight="1">
+      <c r="B53" s="26"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="26"/>
+    </row>
+    <row r="54" spans="2:8" ht="37.25" customHeight="1">
+      <c r="B54" s="18"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="33"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="33"/>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="33"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="33"/>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="33"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="33"/>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1827,16 +2003,16 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="3.296875" customWidth="1"/>
-    <col min="2" max="2" width="31.796875" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.69921875" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" customWidth="1"/>
-    <col min="7" max="7" width="12.296875" customWidth="1"/>
+    <col min="4" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.4140625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="3.296875" customWidth="1"/>
+    <col min="9" max="9" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1">
@@ -1846,7 +2022,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.2" customHeight="1">
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1868,7 +2044,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.2" customHeight="1">
+    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="8"/>
@@ -1886,7 +2062,7 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" ht="10.95" customHeight="1">
+    <row r="4" spans="1:17" ht="11" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1895,7 +2071,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="19.95" customHeight="1">
+    <row r="5" spans="1:17" ht="20" customHeight="1">
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -1918,7 +2094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="19.95" customHeight="1">
+    <row r="6" spans="1:17" ht="20" customHeight="1">
       <c r="B6" s="17" t="s">
         <v>11</v>
       </c>
@@ -1929,7 +2105,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:17" ht="19.95" customHeight="1">
+    <row r="7" spans="1:17" ht="20" customHeight="1">
       <c r="B7" s="18"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1938,7 +2114,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:17" ht="19.95" customHeight="1">
+    <row r="8" spans="1:17" ht="20" customHeight="1">
       <c r="B8" s="18"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -1949,7 +2125,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="19.95" customHeight="1">
+    <row r="9" spans="1:17" ht="20" customHeight="1">
       <c r="B9" s="18"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -1958,7 +2134,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:17" ht="19.95" customHeight="1">
+    <row r="10" spans="1:17" ht="20" customHeight="1">
       <c r="B10" s="18"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1967,7 +2143,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:17" ht="19.95" customHeight="1">
+    <row r="11" spans="1:17" ht="20" customHeight="1">
       <c r="B11" s="17" t="s">
         <v>12</v>
       </c>
@@ -1978,7 +2154,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:17" ht="19.95" customHeight="1">
+    <row r="12" spans="1:17" ht="20" customHeight="1">
       <c r="B12" s="18"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1987,7 +2163,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:17" ht="19.95" customHeight="1">
+    <row r="13" spans="1:17" ht="20" customHeight="1">
       <c r="B13" s="18"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -1996,7 +2172,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:17" ht="19.95" customHeight="1">
+    <row r="14" spans="1:17" ht="20" customHeight="1">
       <c r="B14" s="18"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2005,7 +2181,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="1:17" ht="19.95" customHeight="1">
+    <row r="15" spans="1:17" ht="20" customHeight="1">
       <c r="B15" s="18"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -2014,7 +2190,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:17" ht="19.95" customHeight="1">
+    <row r="16" spans="1:17" ht="20" customHeight="1">
       <c r="B16" s="18"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2023,7 +2199,7 @@
       <c r="G16" s="12"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="2:8" ht="19.95" customHeight="1">
+    <row r="17" spans="2:8" ht="20" customHeight="1">
       <c r="B17" s="17" t="s">
         <v>13</v>
       </c>
@@ -2034,7 +2210,7 @@
       <c r="G17" s="16"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="2:8" ht="19.95" customHeight="1">
+    <row r="18" spans="2:8" ht="20" customHeight="1">
       <c r="B18" s="18"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -2043,7 +2219,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="2:8" ht="19.95" customHeight="1">
+    <row r="19" spans="2:8" ht="20" customHeight="1">
       <c r="B19" s="18"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2052,7 +2228,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="2:8" ht="19.95" customHeight="1">
+    <row r="20" spans="2:8" ht="20" customHeight="1">
       <c r="B20" s="18"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2061,7 +2237,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="2:8" ht="19.95" customHeight="1">
+    <row r="21" spans="2:8" ht="20" customHeight="1">
       <c r="B21" s="18"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -2070,7 +2246,7 @@
       <c r="G21" s="12"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="2:8" ht="19.95" customHeight="1">
+    <row r="22" spans="2:8" ht="20" customHeight="1">
       <c r="B22" s="18"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2079,7 +2255,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="2:8" ht="19.95" customHeight="1">
+    <row r="23" spans="2:8" ht="20" customHeight="1">
       <c r="B23" s="17" t="s">
         <v>14</v>
       </c>
@@ -2090,7 +2266,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="2:8" ht="19.95" customHeight="1">
+    <row r="24" spans="2:8" ht="20" customHeight="1">
       <c r="B24" s="18"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -2099,7 +2275,7 @@
       <c r="G24" s="12"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="2:8" ht="19.95" customHeight="1">
+    <row r="25" spans="2:8" ht="20" customHeight="1">
       <c r="B25" s="18"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -2108,7 +2284,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="2:8" ht="19.95" customHeight="1">
+    <row r="26" spans="2:8" ht="20" customHeight="1">
       <c r="B26" s="18"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2117,7 +2293,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="2:8" ht="19.95" customHeight="1">
+    <row r="27" spans="2:8" ht="20" customHeight="1">
       <c r="B27" s="18"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -2126,7 +2302,7 @@
       <c r="G27" s="12"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="19.95" customHeight="1">
+    <row r="28" spans="2:8" ht="20" customHeight="1">
       <c r="B28" s="18"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -2152,15 +2328,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.296875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.796875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.796875" style="3"/>
+    <col min="1" max="1" width="3.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="88.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="19.95" customHeight="1"/>
+    <row r="1" spans="2:2" ht="20" customHeight="1"/>
     <row r="2" spans="2:2" ht="105" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
plano de ação atualizado
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sp-tech\NocToramento\Documentacao\Documentação do Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/2°Semestre/PI/Noctoramento/Documentacao/Documentação do Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA92C73-644D-428C-9C51-4F89D6D00EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{EEA92C73-644D-428C-9C51-4F89D6D00EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4691C1F5-5A35-40E0-9E6B-03FAE70573C3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Ação" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -209,9 +209,6 @@
     <t xml:space="preserve"> Yuri</t>
   </si>
   <si>
-    <t xml:space="preserve">    Yuri</t>
-  </si>
-  <si>
     <t>BPMN</t>
   </si>
   <si>
@@ -266,6 +263,15 @@
   </si>
   <si>
     <t>Atualizar users stories e proto persona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nathalia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Yuri/Nathalia/Sarabando</t>
   </si>
 </sst>
 </file>
@@ -1073,20 +1079,20 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="44.58203125" customWidth="1"/>
+    <col min="1" max="1" width="3.296875" customWidth="1"/>
+    <col min="2" max="2" width="44.59765625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.58203125" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="42.1640625" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
+    <col min="4" max="5" width="15.69921875" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" customWidth="1"/>
+    <col min="8" max="8" width="42.19921875" customWidth="1"/>
+    <col min="9" max="9" width="3.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
@@ -1101,7 +1107,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="2" spans="1:16" s="6" customFormat="1" ht="22.2" customHeight="1">
       <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
@@ -1122,7 +1128,7 @@
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
     </row>
-    <row r="3" spans="1:16" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="22.2" customHeight="1">
       <c r="B3" s="28" t="s">
         <v>44</v>
       </c>
@@ -1143,7 +1149,7 @@
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" spans="1:16" ht="11" customHeight="1">
+    <row r="4" spans="1:16" ht="10.95" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1152,7 +1158,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:16" ht="20" customHeight="1">
+    <row r="5" spans="1:16" ht="19.95" customHeight="1">
       <c r="B5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="20" customHeight="1">
+    <row r="6" spans="1:16" ht="19.95" customHeight="1">
       <c r="B6" s="21" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1192,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="52.25" customHeight="1">
+    <row r="7" spans="1:16" ht="52.2" customHeight="1">
       <c r="B7" s="11" t="s">
         <v>48</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="39.65" customHeight="1">
+    <row r="8" spans="1:16" ht="39.6" customHeight="1">
       <c r="B8" s="11" t="s">
         <v>34</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="70.25" customHeight="1">
+    <row r="10" spans="1:16" ht="70.2" customHeight="1">
       <c r="B10" s="11" t="s">
         <v>39</v>
       </c>
@@ -1279,13 +1285,13 @@
         <v>41</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="36">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="F11" s="19">
         <v>45381</v>
@@ -1297,7 +1303,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="20" customHeight="1">
+    <row r="12" spans="1:16" ht="19.95" customHeight="1">
       <c r="B12" s="11" t="s">
         <v>46</v>
       </c>
@@ -1318,12 +1324,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="20" customHeight="1">
+    <row r="13" spans="1:16" ht="19.95" customHeight="1">
       <c r="B13" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>21</v>
@@ -1339,7 +1345,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="20" customHeight="1">
+    <row r="14" spans="1:16" ht="19.95" customHeight="1">
       <c r="B14" s="40" t="s">
         <v>3</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="20" customHeight="1">
+    <row r="15" spans="1:16" ht="19.95" customHeight="1">
       <c r="B15" s="21" t="s">
         <v>19</v>
       </c>
@@ -1387,34 +1393,36 @@
         <v>0.5</v>
       </c>
       <c r="F16" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="39" customHeight="1">
       <c r="B17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="E17" s="36">
         <v>0</v>
       </c>
       <c r="F17" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="2:8" ht="39" customHeight="1">
       <c r="B18" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>21</v>
@@ -1423,17 +1431,17 @@
         <v>0</v>
       </c>
       <c r="F18" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="2:8" ht="39.5" customHeight="1">
+    <row r="19" spans="2:8" ht="39.450000000000003" customHeight="1">
       <c r="B19" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>21</v>
@@ -1442,17 +1450,17 @@
         <v>0</v>
       </c>
       <c r="F19" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="2:8" ht="39.5" customHeight="1">
+    <row r="20" spans="2:8" ht="39.450000000000003" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>21</v>
@@ -1461,16 +1469,18 @@
         <v>0</v>
       </c>
       <c r="F20" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="11"/>
     </row>
     <row r="21" spans="2:8" ht="39" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="D21" s="11" t="s">
         <v>21</v>
       </c>
@@ -1478,17 +1488,17 @@
         <v>0</v>
       </c>
       <c r="F21" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="11"/>
     </row>
     <row r="22" spans="2:8" ht="39" customHeight="1">
       <c r="B22" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>21</v>
@@ -1497,17 +1507,17 @@
         <v>0</v>
       </c>
       <c r="F22" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="2:8" ht="67.25" customHeight="1">
+    <row r="23" spans="2:8" ht="67.2" customHeight="1">
       <c r="B23" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>21</v>
@@ -1516,16 +1526,18 @@
         <v>0</v>
       </c>
       <c r="F23" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="18"/>
     </row>
-    <row r="24" spans="2:8" ht="49.25" customHeight="1">
+    <row r="24" spans="2:8" ht="49.2" customHeight="1">
       <c r="B24" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="D24" s="11" t="s">
         <v>21</v>
       </c>
@@ -1533,14 +1545,14 @@
         <v>0.5</v>
       </c>
       <c r="F24" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="2:8" ht="45.65" customHeight="1">
+    <row r="25" spans="2:8" ht="45.6" customHeight="1">
       <c r="B25" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11" t="s">
@@ -1550,14 +1562,14 @@
         <v>0</v>
       </c>
       <c r="F25" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="2:8" ht="49.75" customHeight="1">
+    <row r="26" spans="2:8" ht="49.8" customHeight="1">
       <c r="B26" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
@@ -1567,14 +1579,14 @@
         <v>0</v>
       </c>
       <c r="F26" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="2:8" ht="40.5" customHeight="1">
       <c r="B27" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
@@ -1584,14 +1596,14 @@
         <v>0</v>
       </c>
       <c r="F27" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="36.5" customHeight="1">
+    <row r="28" spans="2:8" ht="36.450000000000003" customHeight="1">
       <c r="B28" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -1601,14 +1613,14 @@
         <v>0</v>
       </c>
       <c r="F28" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G28" s="19"/>
       <c r="H28" s="18"/>
     </row>
     <row r="29" spans="2:8" ht="28.5" customHeight="1">
       <c r="B29" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -1618,17 +1630,17 @@
         <v>0</v>
       </c>
       <c r="F29" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G29" s="19"/>
       <c r="H29" s="18"/>
     </row>
     <row r="30" spans="2:8" ht="40.5" customHeight="1">
       <c r="B30" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>21</v>
@@ -1637,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="19">
-        <v>45390</v>
+        <v>45396</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="18"/>
@@ -1676,7 +1688,7 @@
       <c r="G32" s="31"/>
       <c r="H32" s="21"/>
     </row>
-    <row r="33" spans="2:8" ht="28.25" customHeight="1">
+    <row r="33" spans="2:8" ht="28.2" customHeight="1">
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
@@ -1741,7 +1753,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="2:8" ht="28.25" customHeight="1">
+    <row r="38" spans="2:8" ht="28.2" customHeight="1">
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
@@ -1763,7 +1775,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="18"/>
     </row>
-    <row r="40" spans="2:8" ht="27.65" customHeight="1">
+    <row r="40" spans="2:8" ht="27.6" customHeight="1">
       <c r="B40" s="18"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -1772,7 +1784,7 @@
       <c r="G40" s="19"/>
       <c r="H40" s="18"/>
     </row>
-    <row r="41" spans="2:8" ht="25.25" customHeight="1">
+    <row r="41" spans="2:8" ht="25.2" customHeight="1">
       <c r="B41" s="18"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
@@ -1810,7 +1822,7 @@
       <c r="G44" s="31"/>
       <c r="H44" s="21"/>
     </row>
-    <row r="45" spans="2:8" ht="25.75" customHeight="1">
+    <row r="45" spans="2:8" ht="25.8" customHeight="1">
       <c r="B45" s="26"/>
       <c r="C45" s="27"/>
       <c r="D45" s="27"/>
@@ -1865,7 +1877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="36.65" customHeight="1">
+    <row r="48" spans="2:8" ht="36.6" customHeight="1">
       <c r="B48" s="18" t="s">
         <v>29</v>
       </c>
@@ -1888,7 +1900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="34.75" customHeight="1">
+    <row r="49" spans="2:8" ht="34.799999999999997" customHeight="1">
       <c r="B49" s="26"/>
       <c r="C49" s="27"/>
       <c r="D49" s="27"/>
@@ -1897,7 +1909,7 @@
       <c r="G49" s="32"/>
       <c r="H49" s="26"/>
     </row>
-    <row r="50" spans="2:8" ht="37.75" customHeight="1">
+    <row r="50" spans="2:8" ht="37.799999999999997" customHeight="1">
       <c r="B50" s="26"/>
       <c r="C50" s="27"/>
       <c r="D50" s="27"/>
@@ -1906,7 +1918,7 @@
       <c r="G50" s="32"/>
       <c r="H50" s="26"/>
     </row>
-    <row r="51" spans="2:8" ht="34.25" customHeight="1">
+    <row r="51" spans="2:8" ht="34.200000000000003" customHeight="1">
       <c r="B51" s="18"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -1915,7 +1927,7 @@
       <c r="G51" s="19"/>
       <c r="H51" s="18"/>
     </row>
-    <row r="52" spans="2:8" ht="37.75" customHeight="1">
+    <row r="52" spans="2:8" ht="37.799999999999997" customHeight="1">
       <c r="B52" s="26"/>
       <c r="C52" s="27"/>
       <c r="D52" s="27"/>
@@ -1924,7 +1936,7 @@
       <c r="G52" s="32"/>
       <c r="H52" s="26"/>
     </row>
-    <row r="53" spans="2:8" ht="37.25" customHeight="1">
+    <row r="53" spans="2:8" ht="37.200000000000003" customHeight="1">
       <c r="B53" s="26"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
@@ -1933,7 +1945,7 @@
       <c r="G53" s="32"/>
       <c r="H53" s="26"/>
     </row>
-    <row r="54" spans="2:8" ht="37.25" customHeight="1">
+    <row r="54" spans="2:8" ht="37.200000000000003" customHeight="1">
       <c r="B54" s="18"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -2003,16 +2015,16 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.296875" customWidth="1"/>
+    <col min="2" max="2" width="31.796875" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.4140625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="15.69921875" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
+    <col min="9" max="9" width="3.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1">
@@ -2022,7 +2034,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.2" customHeight="1">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2044,7 +2056,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.2" customHeight="1">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="8"/>
@@ -2062,7 +2074,7 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" ht="11" customHeight="1">
+    <row r="4" spans="1:17" ht="10.95" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2071,7 +2083,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="20" customHeight="1">
+    <row r="5" spans="1:17" ht="19.95" customHeight="1">
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -2094,7 +2106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="20" customHeight="1">
+    <row r="6" spans="1:17" ht="19.95" customHeight="1">
       <c r="B6" s="17" t="s">
         <v>11</v>
       </c>
@@ -2105,7 +2117,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:17" ht="20" customHeight="1">
+    <row r="7" spans="1:17" ht="19.95" customHeight="1">
       <c r="B7" s="18"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -2114,7 +2126,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:17" ht="20" customHeight="1">
+    <row r="8" spans="1:17" ht="19.95" customHeight="1">
       <c r="B8" s="18"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -2125,7 +2137,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="20" customHeight="1">
+    <row r="9" spans="1:17" ht="19.95" customHeight="1">
       <c r="B9" s="18"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -2134,7 +2146,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:17" ht="20" customHeight="1">
+    <row r="10" spans="1:17" ht="19.95" customHeight="1">
       <c r="B10" s="18"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -2143,7 +2155,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:17" ht="20" customHeight="1">
+    <row r="11" spans="1:17" ht="19.95" customHeight="1">
       <c r="B11" s="17" t="s">
         <v>12</v>
       </c>
@@ -2154,7 +2166,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:17" ht="20" customHeight="1">
+    <row r="12" spans="1:17" ht="19.95" customHeight="1">
       <c r="B12" s="18"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -2163,7 +2175,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:17" ht="20" customHeight="1">
+    <row r="13" spans="1:17" ht="19.95" customHeight="1">
       <c r="B13" s="18"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -2172,7 +2184,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:17" ht="20" customHeight="1">
+    <row r="14" spans="1:17" ht="19.95" customHeight="1">
       <c r="B14" s="18"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2181,7 +2193,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="1:17" ht="20" customHeight="1">
+    <row r="15" spans="1:17" ht="19.95" customHeight="1">
       <c r="B15" s="18"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -2190,7 +2202,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:17" ht="20" customHeight="1">
+    <row r="16" spans="1:17" ht="19.95" customHeight="1">
       <c r="B16" s="18"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2199,7 +2211,7 @@
       <c r="G16" s="12"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="2:8" ht="20" customHeight="1">
+    <row r="17" spans="2:8" ht="19.95" customHeight="1">
       <c r="B17" s="17" t="s">
         <v>13</v>
       </c>
@@ -2210,7 +2222,7 @@
       <c r="G17" s="16"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="2:8" ht="20" customHeight="1">
+    <row r="18" spans="2:8" ht="19.95" customHeight="1">
       <c r="B18" s="18"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -2219,7 +2231,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="2:8" ht="20" customHeight="1">
+    <row r="19" spans="2:8" ht="19.95" customHeight="1">
       <c r="B19" s="18"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2228,7 +2240,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="2:8" ht="20" customHeight="1">
+    <row r="20" spans="2:8" ht="19.95" customHeight="1">
       <c r="B20" s="18"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2237,7 +2249,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="2:8" ht="20" customHeight="1">
+    <row r="21" spans="2:8" ht="19.95" customHeight="1">
       <c r="B21" s="18"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -2246,7 +2258,7 @@
       <c r="G21" s="12"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="2:8" ht="20" customHeight="1">
+    <row r="22" spans="2:8" ht="19.95" customHeight="1">
       <c r="B22" s="18"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2255,7 +2267,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="2:8" ht="20" customHeight="1">
+    <row r="23" spans="2:8" ht="19.95" customHeight="1">
       <c r="B23" s="17" t="s">
         <v>14</v>
       </c>
@@ -2266,7 +2278,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="2:8" ht="20" customHeight="1">
+    <row r="24" spans="2:8" ht="19.95" customHeight="1">
       <c r="B24" s="18"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -2275,7 +2287,7 @@
       <c r="G24" s="12"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="2:8" ht="20" customHeight="1">
+    <row r="25" spans="2:8" ht="19.95" customHeight="1">
       <c r="B25" s="18"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -2284,7 +2296,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="2:8" ht="20" customHeight="1">
+    <row r="26" spans="2:8" ht="19.95" customHeight="1">
       <c r="B26" s="18"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2293,7 +2305,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="2:8" ht="20" customHeight="1">
+    <row r="27" spans="2:8" ht="19.95" customHeight="1">
       <c r="B27" s="18"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -2302,7 +2314,7 @@
       <c r="G27" s="12"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="20" customHeight="1">
+    <row r="28" spans="2:8" ht="19.95" customHeight="1">
       <c r="B28" s="18"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -2328,15 +2340,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="3.296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="88.296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="20" customHeight="1"/>
+    <row r="1" spans="2:2" ht="19.95" customHeight="1"/>
     <row r="2" spans="2:2" ht="105" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Atuazação plano de ação
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sp-tech\NocToramento\Documentacao\Documentação do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA92C73-644D-428C-9C51-4F89D6D00EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FFFC93-CCA5-4166-B697-C6F01101E00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plano de Ação'!$B$1:$H$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plano de Ação'!$B$1:$H$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Plano de Ação - EM BRANCO'!$B$1:$H$28</definedName>
     <definedName name="Interval" localSheetId="1">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="Interval">'[1]Return to Work Template'!#REF!</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -266,6 +266,24 @@
   </si>
   <si>
     <t>Atualizar users stories e proto persona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nathalia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualizar Objetivo e justificativa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro Souza </t>
+  </si>
+  <si>
+    <t>Atualizar Diagrama de Solução</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualizar Contexto </t>
   </si>
 </sst>
 </file>
@@ -1070,11 +1088,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -1396,7 +1414,9 @@
       <c r="B17" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="D17" s="11" t="s">
         <v>67</v>
       </c>
@@ -1466,16 +1486,18 @@
       <c r="G20" s="19"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="2:8" ht="39" customHeight="1">
+    <row r="21" spans="2:8" ht="39.5" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="D21" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="19">
         <v>45390</v>
@@ -1483,18 +1505,18 @@
       <c r="G21" s="19"/>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="2:8" ht="39" customHeight="1">
+    <row r="22" spans="2:8" ht="39.5" customHeight="1">
       <c r="B22" s="11" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="19">
         <v>45390</v>
@@ -1502,47 +1524,49 @@
       <c r="G22" s="19"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="2:8" ht="67.25" customHeight="1">
+    <row r="23" spans="2:8" ht="39.5" customHeight="1">
       <c r="B23" s="11" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="36">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F23" s="19">
         <v>45390</v>
       </c>
       <c r="G23" s="19"/>
-      <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="2:8" ht="49.25" customHeight="1">
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="2:8" ht="39" customHeight="1">
       <c r="B24" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="36">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F24" s="19">
         <v>45390</v>
       </c>
       <c r="G24" s="19"/>
-      <c r="H24" s="18"/>
-    </row>
-    <row r="25" spans="2:8" ht="45.65" customHeight="1">
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="2:8" ht="39" customHeight="1">
       <c r="B25" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="11"/>
+        <v>63</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="D25" s="11" t="s">
         <v>21</v>
       </c>
@@ -1553,18 +1577,20 @@
         <v>45390</v>
       </c>
       <c r="G25" s="19"/>
-      <c r="H25" s="18"/>
-    </row>
-    <row r="26" spans="2:8" ht="49.75" customHeight="1">
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="2:8" ht="67.25" customHeight="1">
       <c r="B26" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="11"/>
+        <v>53</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="D26" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="36">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F26" s="19">
         <v>45390</v>
@@ -1572,11 +1598,13 @@
       <c r="G26" s="19"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="2:8" ht="40.5" customHeight="1">
+    <row r="27" spans="2:8" ht="49.25" customHeight="1">
       <c r="B27" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>75</v>
+      </c>
       <c r="D27" s="11" t="s">
         <v>21</v>
       </c>
@@ -1589,9 +1617,9 @@
       <c r="G27" s="19"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="36.5" customHeight="1">
+    <row r="28" spans="2:8" ht="45.65" customHeight="1">
       <c r="B28" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -1606,9 +1634,9 @@
       <c r="G28" s="19"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="2:8" ht="28.5" customHeight="1">
+    <row r="29" spans="2:8" ht="49.75" customHeight="1">
       <c r="B29" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -1625,11 +1653,9 @@
     </row>
     <row r="30" spans="2:8" ht="40.5" customHeight="1">
       <c r="B30" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>69</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
         <v>21</v>
       </c>
@@ -1639,147 +1665,173 @@
       <c r="F30" s="19">
         <v>45390</v>
       </c>
-      <c r="G30" s="12"/>
+      <c r="G30" s="19"/>
       <c r="H30" s="18"/>
     </row>
-    <row r="31" spans="2:8" ht="27" customHeight="1">
-      <c r="B31" s="40" t="s">
+    <row r="31" spans="2:8" ht="36.5" customHeight="1">
+      <c r="B31" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="36">
+        <v>0</v>
+      </c>
+      <c r="F31" s="19">
+        <v>45390</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="2:8" ht="28.5" customHeight="1">
+      <c r="B32" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="36">
+        <v>0</v>
+      </c>
+      <c r="F32" s="19">
+        <v>45390</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B33" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="36">
+        <v>0</v>
+      </c>
+      <c r="F33" s="19">
+        <v>45390</v>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="2:8" ht="27" customHeight="1">
+      <c r="B34" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C34" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D34" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E34" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="41" t="s">
+      <c r="F34" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="41" t="s">
+      <c r="G34" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="40" t="s">
+      <c r="H34" s="40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:8" s="1" customFormat="1" ht="24" customHeight="1">
-      <c r="B32" s="21" t="s">
+    <row r="35" spans="2:8" s="1" customFormat="1" ht="24" customHeight="1">
+      <c r="B35" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="21"/>
-    </row>
-    <row r="33" spans="2:8" ht="28.25" customHeight="1">
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="18"/>
-    </row>
-    <row r="34" spans="2:8" ht="26.4" customHeight="1">
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="36">
-        <v>0.75</v>
-      </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="18"/>
-    </row>
-    <row r="35" spans="2:8" ht="21" customHeight="1">
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="36">
-        <v>0.8</v>
-      </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="18"/>
-    </row>
-    <row r="36" spans="2:8" ht="23.4" customHeight="1">
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="21"/>
+    </row>
+    <row r="36" spans="2:8" ht="28.25" customHeight="1">
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E36" s="36">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="2:8" ht="27" customHeight="1">
+    <row r="37" spans="2:8" ht="26.4" customHeight="1">
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="36">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="2:8" ht="28.25" customHeight="1">
+    <row r="38" spans="2:8" ht="21" customHeight="1">
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E38" s="36">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="2:8" ht="24" customHeight="1">
-      <c r="B39" s="18"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" spans="2:8" ht="23.4" customHeight="1">
+      <c r="B39" s="11"/>
       <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
+      <c r="D39" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="36">
+        <v>0.6</v>
+      </c>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="18"/>
     </row>
-    <row r="40" spans="2:8" ht="27.65" customHeight="1">
-      <c r="B40" s="18"/>
+    <row r="40" spans="2:8" ht="27" customHeight="1">
+      <c r="B40" s="11"/>
       <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
+      <c r="D40" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="36">
+        <v>0</v>
+      </c>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
       <c r="H40" s="18"/>
     </row>
-    <row r="41" spans="2:8" ht="25.25" customHeight="1">
-      <c r="B41" s="18"/>
+    <row r="41" spans="2:8" ht="28.25" customHeight="1">
+      <c r="B41" s="11"/>
       <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
+      <c r="D41" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="36">
+        <v>0</v>
+      </c>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
-      <c r="H41" s="18"/>
+      <c r="H41" s="11"/>
     </row>
     <row r="42" spans="2:8" ht="24" customHeight="1">
       <c r="B42" s="18"/>
@@ -1790,132 +1842,132 @@
       <c r="G42" s="19"/>
       <c r="H42" s="18"/>
     </row>
-    <row r="43" spans="2:8">
-      <c r="B43" s="23" t="s">
+    <row r="43" spans="2:8" ht="27.65" customHeight="1">
+      <c r="B43" s="18"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="2:8" ht="25.25" customHeight="1">
+      <c r="B44" s="18"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="18"/>
+    </row>
+    <row r="45" spans="2:8" ht="24" customHeight="1">
+      <c r="B45" s="18"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="18"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="23"/>
-    </row>
-    <row r="44" spans="2:8">
-      <c r="B44" s="21"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="21"/>
-    </row>
-    <row r="45" spans="2:8" ht="25.75" customHeight="1">
-      <c r="B45" s="26"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="26"/>
-    </row>
-    <row r="46" spans="2:8" ht="39" customHeight="1">
-      <c r="B46" s="26" t="s">
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="23"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="21"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="21"/>
+    </row>
+    <row r="48" spans="2:8" ht="25.75" customHeight="1">
+      <c r="B48" s="26"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="26"/>
+    </row>
+    <row r="49" spans="2:8" ht="39" customHeight="1">
+      <c r="B49" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="C49" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="42">
+      <c r="D49" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="42">
         <v>0.3</v>
       </c>
-      <c r="F46" s="32">
+      <c r="F49" s="32">
         <v>45219</v>
       </c>
-      <c r="G46" s="32">
+      <c r="G49" s="32">
         <v>45222</v>
       </c>
-      <c r="H46" s="26" t="s">
+      <c r="H49" s="26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="33" customHeight="1">
-      <c r="B47" s="26" t="s">
+    <row r="50" spans="2:8" ht="33" customHeight="1">
+      <c r="B50" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="27" t="s">
+      <c r="C50" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E47" s="42">
+      <c r="D50" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="42">
         <v>0.4</v>
       </c>
-      <c r="F47" s="32">
+      <c r="F50" s="32">
         <v>45219</v>
       </c>
-      <c r="G47" s="32">
+      <c r="G50" s="32">
         <v>45222</v>
       </c>
-      <c r="H47" s="26" t="s">
+      <c r="H50" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="36.65" customHeight="1">
-      <c r="B48" s="18" t="s">
+    <row r="51" spans="2:8" ht="36.65" customHeight="1">
+      <c r="B51" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C51" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E48" s="36">
+      <c r="D51" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="36">
         <v>0</v>
       </c>
-      <c r="F48" s="19">
+      <c r="F51" s="19">
         <v>45219</v>
       </c>
-      <c r="G48" s="19">
+      <c r="G51" s="19">
         <v>45222</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H51" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="34.75" customHeight="1">
-      <c r="B49" s="26"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="26"/>
-    </row>
-    <row r="50" spans="2:8" ht="37.75" customHeight="1">
-      <c r="B50" s="26"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="26"/>
-    </row>
-    <row r="51" spans="2:8" ht="34.25" customHeight="1">
-      <c r="B51" s="18"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="18"/>
-    </row>
-    <row r="52" spans="2:8" ht="37.75" customHeight="1">
+    <row r="52" spans="2:8" ht="34.75" customHeight="1">
       <c r="B52" s="26"/>
       <c r="C52" s="27"/>
       <c r="D52" s="27"/>
@@ -1924,7 +1976,7 @@
       <c r="G52" s="32"/>
       <c r="H52" s="26"/>
     </row>
-    <row r="53" spans="2:8" ht="37.25" customHeight="1">
+    <row r="53" spans="2:8" ht="37.75" customHeight="1">
       <c r="B53" s="26"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
@@ -1933,7 +1985,7 @@
       <c r="G53" s="32"/>
       <c r="H53" s="26"/>
     </row>
-    <row r="54" spans="2:8" ht="37.25" customHeight="1">
+    <row r="54" spans="2:8" ht="34.25" customHeight="1">
       <c r="B54" s="18"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -1942,41 +1994,68 @@
       <c r="G54" s="19"/>
       <c r="H54" s="18"/>
     </row>
-    <row r="55" spans="2:8">
-      <c r="B55" s="33"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="33"/>
-    </row>
-    <row r="56" spans="2:8">
-      <c r="B56" s="33"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="33"/>
-    </row>
-    <row r="57" spans="2:8">
-      <c r="B57" s="33"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="33"/>
+    <row r="55" spans="2:8" ht="37.75" customHeight="1">
+      <c r="B55" s="26"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="26"/>
+    </row>
+    <row r="56" spans="2:8" ht="37.25" customHeight="1">
+      <c r="B56" s="26"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="26"/>
+    </row>
+    <row r="57" spans="2:8" ht="37.25" customHeight="1">
+      <c r="B57" s="18"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="18"/>
     </row>
     <row r="58" spans="2:8">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="33"/>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="33"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="33"/>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" s="33"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="35"/>
+      <c r="H60" s="33"/>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1999,7 +2078,7 @@
   </sheetPr>
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualização do Plano de Ação
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sp-tech\NocToramento\Documentacao\Documentação do Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\OneDrive\sptech\Sp-tech\Ads2\LP\lista-03-metodos-PedroHPCSouza-1\Área de Trabalho\NocTotamento\Documentacao\Documentação do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FFFC93-CCA5-4166-B697-C6F01101E00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Ação" sheetId="1" r:id="rId1"/>
@@ -1090,21 +1090,21 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="44.58203125" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="44.625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.58203125" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="42.1640625" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
+    <col min="4" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="8" max="8" width="42.125" customWidth="1"/>
+    <col min="9" max="9" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
@@ -1119,7 +1119,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="2" spans="1:16" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
@@ -1140,7 +1140,7 @@
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
     </row>
-    <row r="3" spans="1:16" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B3" s="28" t="s">
         <v>44</v>
       </c>
@@ -1161,7 +1161,7 @@
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" spans="1:16" ht="11" customHeight="1">
+    <row r="4" spans="1:16" ht="11.1" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1170,7 +1170,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:16" ht="20" customHeight="1">
+    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="20" customHeight="1">
+    <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B6" s="21" t="s">
         <v>16</v>
       </c>
@@ -1204,7 +1204,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="52.25" customHeight="1">
+    <row r="7" spans="1:16" ht="52.35" customHeight="1">
       <c r="B7" s="11" t="s">
         <v>48</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="39.65" customHeight="1">
+    <row r="8" spans="1:16" ht="39.6" customHeight="1">
       <c r="B8" s="11" t="s">
         <v>34</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="44.4" customHeight="1">
+    <row r="9" spans="1:16" ht="44.45" customHeight="1">
       <c r="B9" s="11" t="s">
         <v>36</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="70.25" customHeight="1">
+    <row r="10" spans="1:16" ht="70.349999999999994" customHeight="1">
       <c r="B10" s="11" t="s">
         <v>39</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="20" customHeight="1">
+    <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="11" t="s">
         <v>46</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="20" customHeight="1">
+    <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="11" t="s">
         <v>47</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="20" customHeight="1">
+    <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="40" t="s">
         <v>3</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="20" customHeight="1">
+    <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B15" s="21" t="s">
         <v>19</v>
       </c>
@@ -1407,7 +1407,9 @@
       <c r="F16" s="19">
         <v>45390</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="19">
+        <v>45396</v>
+      </c>
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="39" customHeight="1">
@@ -1426,7 +1428,9 @@
       <c r="F17" s="19">
         <v>45390</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="19">
+        <v>45396</v>
+      </c>
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="2:8" ht="39" customHeight="1">
@@ -1445,10 +1449,12 @@
       <c r="F18" s="19">
         <v>45390</v>
       </c>
-      <c r="G18" s="19"/>
+      <c r="G18" s="19">
+        <v>45396</v>
+      </c>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="2:8" ht="39.5" customHeight="1">
+    <row r="19" spans="2:8" ht="39.6" customHeight="1">
       <c r="B19" s="11" t="s">
         <v>65</v>
       </c>
@@ -1464,10 +1470,12 @@
       <c r="F19" s="19">
         <v>45390</v>
       </c>
-      <c r="G19" s="19"/>
+      <c r="G19" s="19">
+        <v>45396</v>
+      </c>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="2:8" ht="39.5" customHeight="1">
+    <row r="20" spans="2:8" ht="39.6" customHeight="1">
       <c r="B20" s="11" t="s">
         <v>70</v>
       </c>
@@ -1483,10 +1491,12 @@
       <c r="F20" s="19">
         <v>45390</v>
       </c>
-      <c r="G20" s="19"/>
+      <c r="G20" s="19">
+        <v>45396</v>
+      </c>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="2:8" ht="39.5" customHeight="1">
+    <row r="21" spans="2:8" ht="39.6" customHeight="1">
       <c r="B21" s="11" t="s">
         <v>72</v>
       </c>
@@ -1502,10 +1512,12 @@
       <c r="F21" s="19">
         <v>45390</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19">
+        <v>45396</v>
+      </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="2:8" ht="39.5" customHeight="1">
+    <row r="22" spans="2:8" ht="39.6" customHeight="1">
       <c r="B22" s="11" t="s">
         <v>76</v>
       </c>
@@ -1521,10 +1533,12 @@
       <c r="F22" s="19">
         <v>45390</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="19">
+        <v>45396</v>
+      </c>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="2:8" ht="39.5" customHeight="1">
+    <row r="23" spans="2:8" ht="39.6" customHeight="1">
       <c r="B23" s="11" t="s">
         <v>74</v>
       </c>
@@ -1535,12 +1549,14 @@
         <v>21</v>
       </c>
       <c r="E23" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F23" s="19">
         <v>45390</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="19">
+        <v>45396</v>
+      </c>
       <c r="H23" s="11"/>
     </row>
     <row r="24" spans="2:8" ht="39" customHeight="1">
@@ -1557,7 +1573,9 @@
       <c r="F24" s="19">
         <v>45390</v>
       </c>
-      <c r="G24" s="19"/>
+      <c r="G24" s="19">
+        <v>45396</v>
+      </c>
       <c r="H24" s="11"/>
     </row>
     <row r="25" spans="2:8" ht="39" customHeight="1">
@@ -1576,10 +1594,12 @@
       <c r="F25" s="19">
         <v>45390</v>
       </c>
-      <c r="G25" s="19"/>
+      <c r="G25" s="19">
+        <v>45396</v>
+      </c>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="2:8" ht="67.25" customHeight="1">
+    <row r="26" spans="2:8" ht="67.349999999999994" customHeight="1">
       <c r="B26" s="11" t="s">
         <v>53</v>
       </c>
@@ -1595,10 +1615,12 @@
       <c r="F26" s="19">
         <v>45390</v>
       </c>
-      <c r="G26" s="19"/>
+      <c r="G26" s="19">
+        <v>45396</v>
+      </c>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="2:8" ht="49.25" customHeight="1">
+    <row r="27" spans="2:8" ht="49.35" customHeight="1">
       <c r="B27" s="11" t="s">
         <v>68</v>
       </c>
@@ -1609,15 +1631,17 @@
         <v>21</v>
       </c>
       <c r="E27" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="19">
         <v>45390</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="19">
+        <v>45396</v>
+      </c>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="45.65" customHeight="1">
+    <row r="28" spans="2:8" ht="45.6" customHeight="1">
       <c r="B28" s="11" t="s">
         <v>54</v>
       </c>
@@ -1634,7 +1658,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="2:8" ht="49.75" customHeight="1">
+    <row r="29" spans="2:8" ht="49.7" customHeight="1">
       <c r="B29" s="11" t="s">
         <v>55</v>
       </c>
@@ -1668,7 +1692,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="18"/>
     </row>
-    <row r="31" spans="2:8" ht="36.5" customHeight="1">
+    <row r="31" spans="2:8" ht="36.6" customHeight="1">
       <c r="B31" s="11" t="s">
         <v>57</v>
       </c>
@@ -1718,7 +1742,9 @@
       <c r="F33" s="19">
         <v>45390</v>
       </c>
-      <c r="G33" s="12"/>
+      <c r="G33" s="19">
+        <v>45396</v>
+      </c>
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="2:8" ht="27" customHeight="1">
@@ -1755,7 +1781,7 @@
       <c r="G35" s="31"/>
       <c r="H35" s="21"/>
     </row>
-    <row r="36" spans="2:8" ht="28.25" customHeight="1">
+    <row r="36" spans="2:8" ht="28.35" customHeight="1">
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
@@ -1768,7 +1794,7 @@
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="2:8" ht="26.4" customHeight="1">
+    <row r="37" spans="2:8" ht="26.45" customHeight="1">
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
@@ -1794,7 +1820,7 @@
       <c r="G38" s="19"/>
       <c r="H38" s="18"/>
     </row>
-    <row r="39" spans="2:8" ht="23.4" customHeight="1">
+    <row r="39" spans="2:8" ht="23.45" customHeight="1">
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
@@ -1820,7 +1846,7 @@
       <c r="G40" s="19"/>
       <c r="H40" s="18"/>
     </row>
-    <row r="41" spans="2:8" ht="28.25" customHeight="1">
+    <row r="41" spans="2:8" ht="28.35" customHeight="1">
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
@@ -1842,7 +1868,7 @@
       <c r="G42" s="19"/>
       <c r="H42" s="18"/>
     </row>
-    <row r="43" spans="2:8" ht="27.65" customHeight="1">
+    <row r="43" spans="2:8" ht="27.6" customHeight="1">
       <c r="B43" s="18"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
@@ -1851,7 +1877,7 @@
       <c r="G43" s="19"/>
       <c r="H43" s="18"/>
     </row>
-    <row r="44" spans="2:8" ht="25.25" customHeight="1">
+    <row r="44" spans="2:8" ht="25.35" customHeight="1">
       <c r="B44" s="18"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
@@ -1889,7 +1915,7 @@
       <c r="G47" s="31"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="48" spans="2:8" ht="25.75" customHeight="1">
+    <row r="48" spans="2:8" ht="25.7" customHeight="1">
       <c r="B48" s="26"/>
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
@@ -1944,7 +1970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="36.65" customHeight="1">
+    <row r="51" spans="2:8" ht="36.6" customHeight="1">
       <c r="B51" s="18" t="s">
         <v>29</v>
       </c>
@@ -1967,7 +1993,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="34.75" customHeight="1">
+    <row r="52" spans="2:8" ht="34.700000000000003" customHeight="1">
       <c r="B52" s="26"/>
       <c r="C52" s="27"/>
       <c r="D52" s="27"/>
@@ -1976,7 +2002,7 @@
       <c r="G52" s="32"/>
       <c r="H52" s="26"/>
     </row>
-    <row r="53" spans="2:8" ht="37.75" customHeight="1">
+    <row r="53" spans="2:8" ht="37.700000000000003" customHeight="1">
       <c r="B53" s="26"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
@@ -1985,7 +2011,7 @@
       <c r="G53" s="32"/>
       <c r="H53" s="26"/>
     </row>
-    <row r="54" spans="2:8" ht="34.25" customHeight="1">
+    <row r="54" spans="2:8" ht="34.35" customHeight="1">
       <c r="B54" s="18"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -1994,7 +2020,7 @@
       <c r="G54" s="19"/>
       <c r="H54" s="18"/>
     </row>
-    <row r="55" spans="2:8" ht="37.75" customHeight="1">
+    <row r="55" spans="2:8" ht="37.700000000000003" customHeight="1">
       <c r="B55" s="26"/>
       <c r="C55" s="27"/>
       <c r="D55" s="27"/>
@@ -2003,7 +2029,7 @@
       <c r="G55" s="32"/>
       <c r="H55" s="26"/>
     </row>
-    <row r="56" spans="2:8" ht="37.25" customHeight="1">
+    <row r="56" spans="2:8" ht="37.35" customHeight="1">
       <c r="B56" s="26"/>
       <c r="C56" s="27"/>
       <c r="D56" s="27"/>
@@ -2012,7 +2038,7 @@
       <c r="G56" s="32"/>
       <c r="H56" s="26"/>
     </row>
-    <row r="57" spans="2:8" ht="37.25" customHeight="1">
+    <row r="57" spans="2:8" ht="37.35" customHeight="1">
       <c r="B57" s="18"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
@@ -2082,16 +2108,16 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="31.875" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.4140625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
+    <col min="9" max="9" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1">
@@ -2101,7 +2127,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2123,7 +2149,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="8"/>
@@ -2141,7 +2167,7 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" ht="11" customHeight="1">
+    <row r="4" spans="1:17" ht="11.1" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2150,7 +2176,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="20" customHeight="1">
+    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -2173,7 +2199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="20" customHeight="1">
+    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B6" s="17" t="s">
         <v>11</v>
       </c>
@@ -2184,7 +2210,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:17" ht="20" customHeight="1">
+    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="18"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -2193,7 +2219,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:17" ht="20" customHeight="1">
+    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="18"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -2204,7 +2230,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="20" customHeight="1">
+    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B9" s="18"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -2213,7 +2239,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:17" ht="20" customHeight="1">
+    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B10" s="18"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -2222,7 +2248,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:17" ht="20" customHeight="1">
+    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="17" t="s">
         <v>12</v>
       </c>
@@ -2233,7 +2259,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:17" ht="20" customHeight="1">
+    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="18"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -2242,7 +2268,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:17" ht="20" customHeight="1">
+    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="18"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -2251,7 +2277,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:17" ht="20" customHeight="1">
+    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="18"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2260,7 +2286,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="1:17" ht="20" customHeight="1">
+    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B15" s="18"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -2269,7 +2295,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:17" ht="20" customHeight="1">
+    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B16" s="18"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2278,7 +2304,7 @@
       <c r="G16" s="12"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="2:8" ht="20" customHeight="1">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B17" s="17" t="s">
         <v>13</v>
       </c>
@@ -2289,7 +2315,7 @@
       <c r="G17" s="16"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="2:8" ht="20" customHeight="1">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B18" s="18"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -2298,7 +2324,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="2:8" ht="20" customHeight="1">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B19" s="18"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2307,7 +2333,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="2:8" ht="20" customHeight="1">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="18"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -2316,7 +2342,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="2:8" ht="20" customHeight="1">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="18"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -2325,7 +2351,7 @@
       <c r="G21" s="12"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="2:8" ht="20" customHeight="1">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="18"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2334,7 +2360,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="2:8" ht="20" customHeight="1">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="17" t="s">
         <v>14</v>
       </c>
@@ -2345,7 +2371,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="2:8" ht="20" customHeight="1">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="18"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -2354,7 +2380,7 @@
       <c r="G24" s="12"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="2:8" ht="20" customHeight="1">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="18"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -2363,7 +2389,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="2:8" ht="20" customHeight="1">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="18"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2372,7 +2398,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="2:8" ht="20" customHeight="1">
+    <row r="27" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B27" s="18"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -2381,7 +2407,7 @@
       <c r="G27" s="12"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="20" customHeight="1">
+    <row r="28" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B28" s="18"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -2407,15 +2433,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="3.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="88.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="20" customHeight="1"/>
+    <row r="1" spans="2:2" ht="20.100000000000001" customHeight="1"/>
     <row r="2" spans="2:2" ht="105" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
plano de ação atualizada com novas tarefas
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\OneDrive\sptech\Sp-tech\Ads2\LP\lista-03-metodos-PedroHPCSouza-1\Área de Trabalho\NocTotamento\Documentacao\Documentação do Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/2°Semestre/PI/Noctoramento/Documentacao/Documentação do Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{440B9E35-3270-45EA-A673-5638ADA047DD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Ação" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -123,22 +123,13 @@
     <t xml:space="preserve">SPRINT 2C : </t>
   </si>
   <si>
-    <t>Site estátido dashboard</t>
-  </si>
-  <si>
     <t>Todos da equipe</t>
   </si>
   <si>
     <t xml:space="preserve">Criação da dashboard e linkar junto ao login </t>
   </si>
   <si>
-    <t xml:space="preserve">Diagrama de solução </t>
-  </si>
-  <si>
     <t>Terminar a criação do diagrama de solução</t>
-  </si>
-  <si>
-    <t>slides da apresentação</t>
   </si>
   <si>
     <t>Todos  da equipe</t>
@@ -249,41 +240,68 @@
     <t>Tela cadatrar funcionario</t>
   </si>
   <si>
+    <t xml:space="preserve">Tela Redefinir senha </t>
+  </si>
+  <si>
+    <t>Desejavel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualizar DER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuri </t>
+  </si>
+  <si>
+    <t>Atualizar users stories e proto persona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nathalia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualizar Objetivo e justificativa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro Souza </t>
+  </si>
+  <si>
+    <t>Atualizar Diagrama de Solução</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualizar Contexto </t>
+  </si>
+  <si>
     <t xml:space="preserve">
-tela cadatrar maquina </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tela Redefinir senha </t>
-  </si>
-  <si>
-    <t>Desejavel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atualizar DER </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yuri </t>
-  </si>
-  <si>
-    <t>Atualizar users stories e proto persona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nathalia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atualizar Objetivo e justificativa </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedro Souza </t>
-  </si>
-  <si>
-    <t>Atualizar Diagrama de Solução</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atualizar Contexto </t>
+tela cadastrar maquina </t>
+  </si>
+  <si>
+    <t>BD local (mysql)</t>
+  </si>
+  <si>
+    <t>API web data viz</t>
+  </si>
+  <si>
+    <t>Sarabando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tela cadastrar maquina </t>
+  </si>
+  <si>
+    <t>tela cadastrar funcionário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API looca </t>
+  </si>
+  <si>
+    <t>Script de instalação java</t>
+  </si>
+  <si>
+    <t>VM na nuvem + camada de segurança</t>
+  </si>
+  <si>
+    <t>Despriorizado</t>
   </si>
 </sst>
 </file>
@@ -415,7 +433,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +473,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +585,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -711,6 +735,15 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1090,21 +1123,21 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="2" width="44.625" customWidth="1"/>
+    <col min="1" max="1" width="3.3984375" customWidth="1"/>
+    <col min="2" max="2" width="44.59765625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.625" customWidth="1"/>
-    <col min="6" max="6" width="17.625" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
-    <col min="8" max="8" width="42.125" customWidth="1"/>
-    <col min="9" max="9" width="3.375" customWidth="1"/>
+    <col min="4" max="5" width="15.59765625" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12.3984375" customWidth="1"/>
+    <col min="8" max="8" width="42.09765625" customWidth="1"/>
+    <col min="9" max="9" width="3.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
@@ -1142,7 +1175,7 @@
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B3" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="46" t="s">
         <v>18</v>
@@ -1206,10 +1239,10 @@
     </row>
     <row r="7" spans="1:16" ht="52.35" customHeight="1">
       <c r="B7" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>21</v>
@@ -1224,15 +1257,15 @@
         <v>45387</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="39.6" customHeight="1">
       <c r="B8" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>21</v>
@@ -1245,15 +1278,15 @@
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="44.45" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="44.4" customHeight="1">
       <c r="B9" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>21</v>
@@ -1266,15 +1299,15 @@
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="70.349999999999994" customHeight="1">
       <c r="B10" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>21</v>
@@ -1289,15 +1322,15 @@
         <v>45387</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="66" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>21</v>
@@ -1312,12 +1345,12 @@
         <v>45387</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C12" s="43" t="s">
         <v>22</v>
@@ -1333,15 +1366,15 @@
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>21</v>
@@ -1354,7 +1387,7 @@
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1">
@@ -1393,7 +1426,7 @@
     </row>
     <row r="16" spans="1:16" ht="39" customHeight="1">
       <c r="B16" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>22</v>
@@ -1413,32 +1446,34 @@
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="39" customHeight="1">
-      <c r="B17" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="11" t="s">
+      <c r="B17" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="36">
+      <c r="D17" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="53">
         <v>0</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="54">
         <v>45390</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="54">
         <v>45396</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="52" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="39" customHeight="1">
       <c r="B18" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>21</v>
@@ -1456,10 +1491,10 @@
     </row>
     <row r="19" spans="2:8" ht="39.6" customHeight="1">
       <c r="B19" s="11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>21</v>
@@ -1477,10 +1512,10 @@
     </row>
     <row r="20" spans="2:8" ht="39.6" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>21</v>
@@ -1498,10 +1533,10 @@
     </row>
     <row r="21" spans="2:8" ht="39.6" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>21</v>
@@ -1519,10 +1554,10 @@
     </row>
     <row r="22" spans="2:8" ht="39.6" customHeight="1">
       <c r="B22" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>21</v>
@@ -1540,10 +1575,10 @@
     </row>
     <row r="23" spans="2:8" ht="39.6" customHeight="1">
       <c r="B23" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>21</v>
@@ -1561,7 +1596,7 @@
     </row>
     <row r="24" spans="2:8" ht="39" customHeight="1">
       <c r="B24" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
@@ -1580,16 +1615,16 @@
     </row>
     <row r="25" spans="2:8" ht="39" customHeight="1">
       <c r="B25" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="19">
         <v>45390</v>
@@ -1601,10 +1636,10 @@
     </row>
     <row r="26" spans="2:8" ht="67.349999999999994" customHeight="1">
       <c r="B26" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>21</v>
@@ -1622,10 +1657,10 @@
     </row>
     <row r="27" spans="2:8" ht="49.35" customHeight="1">
       <c r="B27" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>21</v>
@@ -1643,7 +1678,7 @@
     </row>
     <row r="28" spans="2:8" ht="45.6" customHeight="1">
       <c r="B28" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -1658,9 +1693,9 @@
       <c r="G28" s="19"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="2:8" ht="49.7" customHeight="1">
+    <row r="29" spans="2:8" ht="49.65" customHeight="1">
       <c r="B29" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -1677,7 +1712,7 @@
     </row>
     <row r="30" spans="2:8" ht="40.5" customHeight="1">
       <c r="B30" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
@@ -1694,7 +1729,7 @@
     </row>
     <row r="31" spans="2:8" ht="36.6" customHeight="1">
       <c r="B31" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
@@ -1711,7 +1746,7 @@
     </row>
     <row r="32" spans="2:8" ht="28.5" customHeight="1">
       <c r="B32" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
@@ -1728,10 +1763,10 @@
     </row>
     <row r="33" spans="2:8" ht="40.5" customHeight="1">
       <c r="B33" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>21</v>
@@ -1782,8 +1817,12 @@
       <c r="H35" s="21"/>
     </row>
     <row r="36" spans="2:8" ht="28.35" customHeight="1">
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
+      <c r="B36" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="D36" s="11" t="s">
         <v>21</v>
       </c>
@@ -1794,9 +1833,13 @@
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="2:8" ht="26.45" customHeight="1">
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+    <row r="37" spans="2:8" ht="26.4" customHeight="1">
+      <c r="B37" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="D37" s="11" t="s">
         <v>21</v>
       </c>
@@ -1808,10 +1851,14 @@
       <c r="H37" s="18"/>
     </row>
     <row r="38" spans="2:8" ht="21" customHeight="1">
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
+      <c r="B38" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="D38" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E38" s="36">
         <v>0.8</v>
@@ -1820,9 +1867,13 @@
       <c r="G38" s="19"/>
       <c r="H38" s="18"/>
     </row>
-    <row r="39" spans="2:8" ht="23.45" customHeight="1">
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+    <row r="39" spans="2:8" ht="23.4" customHeight="1">
+      <c r="B39" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="D39" s="11" t="s">
         <v>21</v>
       </c>
@@ -1834,8 +1885,12 @@
       <c r="H39" s="18"/>
     </row>
     <row r="40" spans="2:8" ht="27" customHeight="1">
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
+      <c r="B40" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D40" s="11" t="s">
         <v>21</v>
       </c>
@@ -1847,8 +1902,12 @@
       <c r="H40" s="18"/>
     </row>
     <row r="41" spans="2:8" ht="28.35" customHeight="1">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+      <c r="B41" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D41" s="11" t="s">
         <v>21</v>
       </c>
@@ -1860,27 +1919,39 @@
       <c r="H41" s="11"/>
     </row>
     <row r="42" spans="2:8" ht="24" customHeight="1">
-      <c r="B42" s="18"/>
+      <c r="B42" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
+      <c r="D42" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="E42" s="11"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
       <c r="H42" s="18"/>
     </row>
     <row r="43" spans="2:8" ht="27.6" customHeight="1">
-      <c r="B43" s="18"/>
+      <c r="B43" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="D43" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="E43" s="11"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
       <c r="H43" s="18"/>
     </row>
     <row r="44" spans="2:8" ht="25.35" customHeight="1">
-      <c r="B44" s="18"/>
+      <c r="B44" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
+      <c r="D44" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="E44" s="11"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
@@ -1915,7 +1986,7 @@
       <c r="G47" s="31"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="48" spans="2:8" ht="25.7" customHeight="1">
+    <row r="48" spans="2:8" ht="25.65" customHeight="1">
       <c r="B48" s="26"/>
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
@@ -1925,11 +1996,9 @@
       <c r="H48" s="26"/>
     </row>
     <row r="49" spans="2:8" ht="39" customHeight="1">
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="26"/>
+      <c r="C49" s="27" t="s">
         <v>24</v>
-      </c>
-      <c r="C49" s="27" t="s">
-        <v>25</v>
       </c>
       <c r="D49" s="27" t="s">
         <v>21</v>
@@ -1944,15 +2013,13 @@
         <v>45222</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="33" customHeight="1">
-      <c r="B50" s="26" t="s">
-        <v>27</v>
-      </c>
+      <c r="B50" s="26"/>
       <c r="C50" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D50" s="27" t="s">
         <v>21</v>
@@ -1967,15 +2034,13 @@
         <v>45222</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="36.6" customHeight="1">
-      <c r="B51" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="B51" s="18"/>
       <c r="C51" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>21</v>
@@ -1990,10 +2055,10 @@
         <v>45222</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" ht="34.700000000000003" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="34.65" customHeight="1">
       <c r="B52" s="26"/>
       <c r="C52" s="27"/>
       <c r="D52" s="27"/>
@@ -2002,7 +2067,7 @@
       <c r="G52" s="32"/>
       <c r="H52" s="26"/>
     </row>
-    <row r="53" spans="2:8" ht="37.700000000000003" customHeight="1">
+    <row r="53" spans="2:8" ht="37.65" customHeight="1">
       <c r="B53" s="26"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
@@ -2020,7 +2085,7 @@
       <c r="G54" s="19"/>
       <c r="H54" s="18"/>
     </row>
-    <row r="55" spans="2:8" ht="37.700000000000003" customHeight="1">
+    <row r="55" spans="2:8" ht="37.65" customHeight="1">
       <c r="B55" s="26"/>
       <c r="C55" s="27"/>
       <c r="D55" s="27"/>
@@ -2108,16 +2173,16 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="2" width="31.875" customWidth="1"/>
+    <col min="1" max="1" width="3.3984375" customWidth="1"/>
+    <col min="2" max="2" width="31.8984375" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.625" customWidth="1"/>
-    <col min="6" max="6" width="13.375" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="4" max="5" width="15.59765625" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.3984375" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="3.375" customWidth="1"/>
+    <col min="9" max="9" width="3.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1">
@@ -2227,7 +2292,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
@@ -2433,12 +2498,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="3"/>
+    <col min="1" max="1" width="3.3984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="88.3984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.8984375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
bd com tabela de cadastro com rotas web data viz
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/2°Semestre/PI/Noctoramento/Documentacao/Documentação do Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{440B9E35-3270-45EA-A673-5638ADA047DD}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6A1B909-47F4-449E-836F-2A9D0B93C269}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>Despriorizado</t>
+  </si>
+  <si>
+    <t>BD VM</t>
   </si>
 </sst>
 </file>
@@ -712,6 +715,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,15 +747,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -793,6 +796,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1125,7 +1132,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1142,24 +1149,24 @@
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" spans="1:16" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="38"/>
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
@@ -1177,14 +1184,14 @@
       <c r="B3" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="51"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1446,25 +1453,25 @@
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="39" customHeight="1">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="53">
+      <c r="E17" s="45">
         <v>0</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="46">
         <v>45390</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="46">
         <v>45396</v>
       </c>
-      <c r="H17" s="52" t="s">
+      <c r="H17" s="44" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1922,7 +1929,9 @@
       <c r="B42" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="11"/>
+      <c r="C42" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="D42" s="11" t="s">
         <v>21</v>
       </c>
@@ -1935,7 +1944,9 @@
       <c r="B43" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="11"/>
+      <c r="C43" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="D43" s="11" t="s">
         <v>21</v>
       </c>
@@ -1958,7 +1969,9 @@
       <c r="H44" s="18"/>
     </row>
     <row r="45" spans="2:8" ht="24" customHeight="1">
-      <c r="B45" s="18"/>
+      <c r="B45" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>

</xml_diff>

<commit_message>
Plano de ação att
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/2°Semestre/PI/Noctoramento/Documentacao/Documentação do Projeto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sseve\Desktop\FACULDADE\Projetos\Noctoramento\Documentacao\Documentação do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6A1B909-47F4-449E-836F-2A9D0B93C269}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14622DF2-7ED9-4D32-ABE3-279FC8D0F133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Ação" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="79">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -121,21 +121,6 @@
   </si>
   <si>
     <t xml:space="preserve">SPRINT 2C : </t>
-  </si>
-  <si>
-    <t>Todos da equipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criação da dashboard e linkar junto ao login </t>
-  </si>
-  <si>
-    <t>Terminar a criação do diagrama de solução</t>
-  </si>
-  <si>
-    <t>Todos  da equipe</t>
-  </si>
-  <si>
-    <t>Fazer os slides para a apresentação</t>
   </si>
   <si>
     <t xml:space="preserve">Essencial </t>
@@ -796,10 +781,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1131,20 +1112,20 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49:H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" customWidth="1"/>
-    <col min="2" max="2" width="44.59765625" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="44.625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.59765625" customWidth="1"/>
-    <col min="6" max="6" width="17.59765625" customWidth="1"/>
-    <col min="7" max="7" width="12.3984375" customWidth="1"/>
-    <col min="8" max="8" width="42.09765625" customWidth="1"/>
-    <col min="9" max="9" width="3.3984375" customWidth="1"/>
+    <col min="4" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="8" max="8" width="42.125" customWidth="1"/>
+    <col min="9" max="9" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
@@ -1182,7 +1163,7 @@
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B3" s="28" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>18</v>
@@ -1246,10 +1227,10 @@
     </row>
     <row r="7" spans="1:16" ht="52.35" customHeight="1">
       <c r="B7" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>21</v>
@@ -1264,15 +1245,15 @@
         <v>45387</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="39.6" customHeight="1">
       <c r="B8" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>21</v>
@@ -1285,15 +1266,15 @@
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="44.4" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="44.45" customHeight="1">
       <c r="B9" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>21</v>
@@ -1306,15 +1287,15 @@
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="70.349999999999994" customHeight="1">
       <c r="B10" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>21</v>
@@ -1329,15 +1310,15 @@
         <v>45387</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="66" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>21</v>
@@ -1352,12 +1333,12 @@
         <v>45387</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="43" t="s">
         <v>22</v>
@@ -1373,15 +1354,15 @@
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>21</v>
@@ -1394,7 +1375,7 @@
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1">
@@ -1433,7 +1414,7 @@
     </row>
     <row r="16" spans="1:16" ht="39" customHeight="1">
       <c r="B16" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>22</v>
@@ -1454,13 +1435,13 @@
     </row>
     <row r="17" spans="2:8" ht="39" customHeight="1">
       <c r="B17" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="44" t="s">
-        <v>67</v>
-      </c>
       <c r="D17" s="44" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E17" s="45">
         <v>0</v>
@@ -1472,15 +1453,15 @@
         <v>45396</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="39" customHeight="1">
       <c r="B18" s="11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>21</v>
@@ -1498,10 +1479,10 @@
     </row>
     <row r="19" spans="2:8" ht="39.6" customHeight="1">
       <c r="B19" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>21</v>
@@ -1519,10 +1500,10 @@
     </row>
     <row r="20" spans="2:8" ht="39.6" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>21</v>
@@ -1540,10 +1521,10 @@
     </row>
     <row r="21" spans="2:8" ht="39.6" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>21</v>
@@ -1561,10 +1542,10 @@
     </row>
     <row r="22" spans="2:8" ht="39.6" customHeight="1">
       <c r="B22" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>21</v>
@@ -1582,10 +1563,10 @@
     </row>
     <row r="23" spans="2:8" ht="39.6" customHeight="1">
       <c r="B23" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>21</v>
@@ -1603,7 +1584,7 @@
     </row>
     <row r="24" spans="2:8" ht="39" customHeight="1">
       <c r="B24" s="11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
@@ -1622,10 +1603,10 @@
     </row>
     <row r="25" spans="2:8" ht="39" customHeight="1">
       <c r="B25" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>21</v>
@@ -1643,10 +1624,10 @@
     </row>
     <row r="26" spans="2:8" ht="67.349999999999994" customHeight="1">
       <c r="B26" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>21</v>
@@ -1664,10 +1645,10 @@
     </row>
     <row r="27" spans="2:8" ht="49.35" customHeight="1">
       <c r="B27" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>21</v>
@@ -1685,7 +1666,7 @@
     </row>
     <row r="28" spans="2:8" ht="45.6" customHeight="1">
       <c r="B28" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
@@ -1700,9 +1681,9 @@
       <c r="G28" s="19"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="2:8" ht="49.65" customHeight="1">
+    <row r="29" spans="2:8" ht="49.7" customHeight="1">
       <c r="B29" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
@@ -1719,7 +1700,7 @@
     </row>
     <row r="30" spans="2:8" ht="40.5" customHeight="1">
       <c r="B30" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
@@ -1736,7 +1717,7 @@
     </row>
     <row r="31" spans="2:8" ht="36.6" customHeight="1">
       <c r="B31" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
@@ -1753,7 +1734,7 @@
     </row>
     <row r="32" spans="2:8" ht="28.5" customHeight="1">
       <c r="B32" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
@@ -1770,10 +1751,10 @@
     </row>
     <row r="33" spans="2:8" ht="40.5" customHeight="1">
       <c r="B33" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>21</v>
@@ -1825,10 +1806,10 @@
     </row>
     <row r="36" spans="2:8" ht="28.35" customHeight="1">
       <c r="B36" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>21</v>
@@ -1840,12 +1821,12 @@
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="2:8" ht="26.4" customHeight="1">
+    <row r="37" spans="2:8" ht="26.45" customHeight="1">
       <c r="B37" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>21</v>
@@ -1859,13 +1840,13 @@
     </row>
     <row r="38" spans="2:8" ht="21" customHeight="1">
       <c r="B38" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E38" s="36">
         <v>0.8</v>
@@ -1874,9 +1855,9 @@
       <c r="G38" s="19"/>
       <c r="H38" s="18"/>
     </row>
-    <row r="39" spans="2:8" ht="23.4" customHeight="1">
+    <row r="39" spans="2:8" ht="23.45" customHeight="1">
       <c r="B39" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>22</v>
@@ -1885,7 +1866,7 @@
         <v>21</v>
       </c>
       <c r="E39" s="36">
-        <v>0.6</v>
+        <v>0.95</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
@@ -1893,10 +1874,10 @@
     </row>
     <row r="40" spans="2:8" ht="27" customHeight="1">
       <c r="B40" s="11" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>21</v>
@@ -1910,10 +1891,10 @@
     </row>
     <row r="41" spans="2:8" ht="28.35" customHeight="1">
       <c r="B41" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>21</v>
@@ -1927,54 +1908,68 @@
     </row>
     <row r="42" spans="2:8" ht="24" customHeight="1">
       <c r="B42" s="11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="11"/>
+      <c r="E42" s="36">
+        <v>0</v>
+      </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
       <c r="H42" s="18"/>
     </row>
     <row r="43" spans="2:8" ht="27.6" customHeight="1">
       <c r="B43" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E43" s="11"/>
+      <c r="E43" s="36">
+        <v>0</v>
+      </c>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
       <c r="H43" s="18"/>
     </row>
     <row r="44" spans="2:8" ht="25.35" customHeight="1">
       <c r="B44" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C44" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="D44" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="11"/>
+      <c r="E44" s="36">
+        <v>0</v>
+      </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
       <c r="H44" s="18"/>
     </row>
     <row r="45" spans="2:8" ht="24" customHeight="1">
       <c r="B45" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
+        <v>78</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="36">
+        <v>0.3</v>
+      </c>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
       <c r="H45" s="18"/>
@@ -1999,7 +1994,7 @@
       <c r="G47" s="31"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="48" spans="2:8" ht="25.65" customHeight="1">
+    <row r="48" spans="2:8" ht="25.7" customHeight="1">
       <c r="B48" s="26"/>
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
@@ -2010,68 +2005,32 @@
     </row>
     <row r="49" spans="2:8" ht="39" customHeight="1">
       <c r="B49" s="26"/>
-      <c r="C49" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E49" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="F49" s="32">
-        <v>45219</v>
-      </c>
-      <c r="G49" s="32">
-        <v>45222</v>
-      </c>
-      <c r="H49" s="26" t="s">
-        <v>25</v>
-      </c>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="26"/>
     </row>
     <row r="50" spans="2:8" ht="33" customHeight="1">
       <c r="B50" s="26"/>
-      <c r="C50" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E50" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="F50" s="32">
-        <v>45219</v>
-      </c>
-      <c r="G50" s="32">
-        <v>45222</v>
-      </c>
-      <c r="H50" s="26" t="s">
-        <v>26</v>
-      </c>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="26"/>
     </row>
     <row r="51" spans="2:8" ht="36.6" customHeight="1">
       <c r="B51" s="18"/>
-      <c r="C51" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E51" s="36">
-        <v>0</v>
-      </c>
-      <c r="F51" s="19">
-        <v>45219</v>
-      </c>
-      <c r="G51" s="19">
-        <v>45222</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" ht="34.65" customHeight="1">
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="2:8" ht="34.700000000000003" customHeight="1">
       <c r="B52" s="26"/>
       <c r="C52" s="27"/>
       <c r="D52" s="27"/>
@@ -2080,7 +2039,7 @@
       <c r="G52" s="32"/>
       <c r="H52" s="26"/>
     </row>
-    <row r="53" spans="2:8" ht="37.65" customHeight="1">
+    <row r="53" spans="2:8" ht="37.700000000000003" customHeight="1">
       <c r="B53" s="26"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
@@ -2098,7 +2057,7 @@
       <c r="G54" s="19"/>
       <c r="H54" s="18"/>
     </row>
-    <row r="55" spans="2:8" ht="37.65" customHeight="1">
+    <row r="55" spans="2:8" ht="37.700000000000003" customHeight="1">
       <c r="B55" s="26"/>
       <c r="C55" s="27"/>
       <c r="D55" s="27"/>
@@ -2186,16 +2145,16 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" customWidth="1"/>
-    <col min="2" max="2" width="31.8984375" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="31.875" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.59765625" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" customWidth="1"/>
-    <col min="7" max="7" width="12.3984375" customWidth="1"/>
+    <col min="4" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="3.3984375" customWidth="1"/>
+    <col min="9" max="9" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1">
@@ -2305,7 +2264,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
@@ -2511,12 +2470,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.3984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.8984375" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.8984375" style="3"/>
+    <col min="1" max="1" width="3.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="88.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
Ata do dia 16/05 e Plano de ação
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sseve\Desktop\FACULDADE\Projetos\Noctoramento\Documentacao\Documentação do Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c7235aa8075ae8b/Área de Trabalho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14622DF2-7ED9-4D32-ABE3-279FC8D0F133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42D6CC88-4966-46F4-B7AA-814279061F1A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Ação" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="109">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t xml:space="preserve">SPRINT 2B : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPRINT  2D: </t>
   </si>
   <si>
     <t>Essencial</t>
@@ -289,7 +286,100 @@
     <t>Despriorizado</t>
   </si>
   <si>
-    <t>BD VM</t>
+    <t>Alertas automáticos</t>
+  </si>
+  <si>
+    <t>Interação com Slack</t>
+  </si>
+  <si>
+    <t>Jar Grupo Completo</t>
+  </si>
+  <si>
+    <t>Diagrama de classes</t>
+  </si>
+  <si>
+    <t>Dashs Dinâmicas</t>
+  </si>
+  <si>
+    <t>Atualizar Script de Instalação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPRINT  3B: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPRINT  3A: </t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Atualizar Documentação (Versão final)</t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>Atualizar DER (versão final)</t>
+  </si>
+  <si>
+    <t>Garantir Padrozinação do site</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Gabriela</t>
+  </si>
+  <si>
+    <t>Nathalia - Luiz</t>
+  </si>
+  <si>
+    <t>Conexão CRUD - Banco</t>
+  </si>
+  <si>
+    <t>Luiz</t>
+  </si>
+  <si>
+    <t>Yuri</t>
+  </si>
+  <si>
+    <t>Inovação (Completa)</t>
+  </si>
+  <si>
+    <t>Atualizar CRUD</t>
+  </si>
+  <si>
+    <t>Atualizar visão geral máquinas</t>
+  </si>
+  <si>
+    <t>Gabriela - Nathalia</t>
+  </si>
+  <si>
+    <t>Pedro Henrique - Sarabando</t>
+  </si>
+  <si>
+    <t>Requisitos: Henrança e Relacionamento de classes</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Feito e validado com a Caramico</t>
+  </si>
+  <si>
+    <t>Nathalia</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Andamento</t>
+  </si>
+  <si>
+    <t>Versão final, sem mudanças após</t>
   </si>
 </sst>
 </file>
@@ -1109,23 +1199,23 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49:H51"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="2" width="44.625" customWidth="1"/>
+    <col min="1" max="1" width="3.3984375" customWidth="1"/>
+    <col min="2" max="2" width="44.59765625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.625" customWidth="1"/>
-    <col min="6" max="6" width="17.625" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
-    <col min="8" max="8" width="42.125" customWidth="1"/>
-    <col min="9" max="9" width="3.375" customWidth="1"/>
+    <col min="4" max="5" width="15.59765625" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12.3984375" customWidth="1"/>
+    <col min="8" max="8" width="42.09765625" customWidth="1"/>
+    <col min="9" max="9" width="3.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
@@ -1163,7 +1253,7 @@
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B3" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>18</v>
@@ -1227,13 +1317,13 @@
     </row>
     <row r="7" spans="1:16" ht="52.35" customHeight="1">
       <c r="B7" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="36">
         <v>1</v>
@@ -1245,18 +1335,18 @@
         <v>45387</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="39.6" customHeight="1">
       <c r="B8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="36">
         <v>1</v>
@@ -1266,18 +1356,18 @@
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="44.4" customHeight="1">
+      <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="44.45" customHeight="1">
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="36">
         <v>0.9</v>
@@ -1287,18 +1377,18 @@
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="70.349999999999994" customHeight="1">
       <c r="B10" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="36">
         <v>1</v>
@@ -1310,18 +1400,18 @@
         <v>45387</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="66" customHeight="1">
       <c r="B11" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="36">
         <v>0.15</v>
@@ -1333,18 +1423,18 @@
         <v>45387</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="36">
         <v>0.5</v>
@@ -1354,18 +1444,18 @@
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="36">
         <v>0.9</v>
@@ -1375,7 +1465,7 @@
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1">
@@ -1414,13 +1504,13 @@
     </row>
     <row r="16" spans="1:16" ht="39" customHeight="1">
       <c r="B16" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="36">
         <v>0.5</v>
@@ -1435,13 +1525,13 @@
     </row>
     <row r="17" spans="2:8" ht="39" customHeight="1">
       <c r="B17" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="44" t="s">
         <v>57</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>58</v>
       </c>
       <c r="E17" s="45">
         <v>0</v>
@@ -1453,18 +1543,18 @@
         <v>45396</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="39" customHeight="1">
       <c r="B18" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="36">
         <v>0</v>
@@ -1479,13 +1569,13 @@
     </row>
     <row r="19" spans="2:8" ht="39.6" customHeight="1">
       <c r="B19" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="36">
         <v>0</v>
@@ -1500,13 +1590,13 @@
     </row>
     <row r="20" spans="2:8" ht="39.6" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="36">
         <v>0</v>
@@ -1521,13 +1611,13 @@
     </row>
     <row r="21" spans="2:8" ht="39.6" customHeight="1">
       <c r="B21" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="D21" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="36">
         <v>1</v>
@@ -1542,13 +1632,13 @@
     </row>
     <row r="22" spans="2:8" ht="39.6" customHeight="1">
       <c r="B22" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="36">
         <v>1</v>
@@ -1563,13 +1653,13 @@
     </row>
     <row r="23" spans="2:8" ht="39.6" customHeight="1">
       <c r="B23" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="36">
         <v>1</v>
@@ -1584,11 +1674,11 @@
     </row>
     <row r="24" spans="2:8" ht="39" customHeight="1">
       <c r="B24" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E24" s="36">
         <v>0</v>
@@ -1603,13 +1693,13 @@
     </row>
     <row r="25" spans="2:8" ht="39" customHeight="1">
       <c r="B25" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25" s="36">
         <v>1</v>
@@ -1624,13 +1714,13 @@
     </row>
     <row r="26" spans="2:8" ht="67.349999999999994" customHeight="1">
       <c r="B26" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="36">
         <v>0.3</v>
@@ -1645,13 +1735,13 @@
     </row>
     <row r="27" spans="2:8" ht="49.35" customHeight="1">
       <c r="B27" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E27" s="36">
         <v>1</v>
@@ -1666,11 +1756,11 @@
     </row>
     <row r="28" spans="2:8" ht="45.6" customHeight="1">
       <c r="B28" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E28" s="36">
         <v>0</v>
@@ -1681,13 +1771,13 @@
       <c r="G28" s="19"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="2:8" ht="49.7" customHeight="1">
+    <row r="29" spans="2:8" ht="49.65" customHeight="1">
       <c r="B29" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="36">
         <v>0</v>
@@ -1700,11 +1790,11 @@
     </row>
     <row r="30" spans="2:8" ht="40.5" customHeight="1">
       <c r="B30" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E30" s="36">
         <v>0</v>
@@ -1717,11 +1807,11 @@
     </row>
     <row r="31" spans="2:8" ht="36.6" customHeight="1">
       <c r="B31" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" s="36">
         <v>0</v>
@@ -1734,11 +1824,11 @@
     </row>
     <row r="32" spans="2:8" ht="28.5" customHeight="1">
       <c r="B32" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E32" s="36">
         <v>0</v>
@@ -1751,13 +1841,13 @@
     </row>
     <row r="33" spans="2:8" ht="40.5" customHeight="1">
       <c r="B33" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E33" s="36">
         <v>0</v>
@@ -1795,7 +1885,7 @@
     </row>
     <row r="35" spans="2:8" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="B35" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="30"/>
       <c r="D35" s="30"/>
@@ -1806,13 +1896,13 @@
     </row>
     <row r="36" spans="2:8" ht="28.35" customHeight="1">
       <c r="B36" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E36" s="36">
         <v>0.5</v>
@@ -1821,15 +1911,15 @@
       <c r="G36" s="19"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="2:8" ht="26.45" customHeight="1">
+    <row r="37" spans="2:8" ht="26.4" customHeight="1">
       <c r="B37" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E37" s="36">
         <v>0.75</v>
@@ -1840,13 +1930,13 @@
     </row>
     <row r="38" spans="2:8" ht="21" customHeight="1">
       <c r="B38" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E38" s="36">
         <v>0.8</v>
@@ -1855,18 +1945,18 @@
       <c r="G38" s="19"/>
       <c r="H38" s="18"/>
     </row>
-    <row r="39" spans="2:8" ht="23.45" customHeight="1">
+    <row r="39" spans="2:8" ht="23.4" customHeight="1">
       <c r="B39" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E39" s="36">
-        <v>0.95</v>
+        <v>0.6</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
@@ -1874,13 +1964,13 @@
     </row>
     <row r="40" spans="2:8" ht="27" customHeight="1">
       <c r="B40" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E40" s="36">
         <v>0</v>
@@ -1891,13 +1981,13 @@
     </row>
     <row r="41" spans="2:8" ht="28.35" customHeight="1">
       <c r="B41" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E41" s="36">
         <v>0</v>
@@ -1908,75 +1998,55 @@
     </row>
     <row r="42" spans="2:8" ht="24" customHeight="1">
       <c r="B42" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>62</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="36">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E42" s="11"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
       <c r="H42" s="18"/>
     </row>
     <row r="43" spans="2:8" ht="27.6" customHeight="1">
       <c r="B43" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>62</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="36">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E43" s="11"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
       <c r="H43" s="18"/>
     </row>
     <row r="44" spans="2:8" ht="25.35" customHeight="1">
       <c r="B44" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>22</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C44" s="11"/>
       <c r="D44" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="36">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E44" s="11"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
       <c r="H44" s="18"/>
     </row>
     <row r="45" spans="2:8" ht="24" customHeight="1">
-      <c r="B45" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="36">
-        <v>0.3</v>
-      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="23" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="24"/>
@@ -1994,131 +2064,370 @@
       <c r="G47" s="31"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="48" spans="2:8" ht="25.7" customHeight="1">
-      <c r="B48" s="26"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="26"/>
+    <row r="48" spans="2:8" ht="25.65" customHeight="1">
+      <c r="B48" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="49" spans="2:8" ht="39" customHeight="1">
-      <c r="B49" s="26"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
+      <c r="B49" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="F49" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G49" s="32">
+        <v>45413</v>
+      </c>
       <c r="H49" s="26"/>
     </row>
     <row r="50" spans="2:8" ht="33" customHeight="1">
-      <c r="B50" s="26"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
+      <c r="B50" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G50" s="32">
+        <v>45413</v>
+      </c>
       <c r="H50" s="26"/>
     </row>
     <row r="51" spans="2:8" ht="36.6" customHeight="1">
-      <c r="B51" s="18"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="18"/>
-    </row>
-    <row r="52" spans="2:8" ht="34.700000000000003" customHeight="1">
-      <c r="B52" s="26"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="26"/>
-    </row>
-    <row r="53" spans="2:8" ht="37.700000000000003" customHeight="1">
-      <c r="B53" s="26"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="26"/>
+      <c r="B51" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="19">
+        <v>45429</v>
+      </c>
+      <c r="G51" s="19">
+        <v>45413</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="34.65" customHeight="1">
+      <c r="B52" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F52" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G52" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H52" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="37.65" customHeight="1">
+      <c r="B53" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" s="19">
+        <v>45429</v>
+      </c>
+      <c r="G53" s="19">
+        <v>45413</v>
+      </c>
+      <c r="H53" s="26" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="54" spans="2:8" ht="34.35" customHeight="1">
-      <c r="B54" s="18"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="18"/>
-    </row>
-    <row r="55" spans="2:8" ht="37.700000000000003" customHeight="1">
-      <c r="B55" s="26"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
+      <c r="B54" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" s="19">
+        <v>45429</v>
+      </c>
+      <c r="G54" s="19">
+        <v>45413</v>
+      </c>
+      <c r="H54" s="26"/>
+    </row>
+    <row r="55" spans="2:8" ht="37.65" customHeight="1">
+      <c r="B55" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G55" s="32">
+        <v>45413</v>
+      </c>
       <c r="H55" s="26"/>
     </row>
     <row r="56" spans="2:8" ht="37.35" customHeight="1">
-      <c r="B56" s="26"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="26"/>
-    </row>
-    <row r="57" spans="2:8" ht="37.35" customHeight="1">
-      <c r="B57" s="18"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="18"/>
-    </row>
-    <row r="58" spans="2:8">
-      <c r="B58" s="33"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="33"/>
-    </row>
-    <row r="59" spans="2:8">
-      <c r="B59" s="33"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="33"/>
-    </row>
-    <row r="60" spans="2:8">
-      <c r="B60" s="33"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="33"/>
-    </row>
-    <row r="61" spans="2:8">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+      <c r="B56" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F56" s="19">
+        <v>45429</v>
+      </c>
+      <c r="G56" s="19">
+        <v>45413</v>
+      </c>
+      <c r="H56" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="34.200000000000003" customHeight="1">
+      <c r="B57" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F57" s="19">
+        <v>45429</v>
+      </c>
+      <c r="G57" s="19">
+        <v>45413</v>
+      </c>
+      <c r="H57" s="26"/>
+    </row>
+    <row r="58" spans="2:8" ht="36.6" customHeight="1">
+      <c r="B58" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F58" s="19">
+        <v>45429</v>
+      </c>
+      <c r="G58" s="19">
+        <v>45413</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="37.799999999999997" customHeight="1">
+      <c r="B59" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G59" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H59" s="26"/>
+    </row>
+    <row r="60" spans="2:8" ht="33" customHeight="1">
+      <c r="B60" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F60" s="19">
+        <v>45429</v>
+      </c>
+      <c r="G60" s="19">
+        <v>45413</v>
+      </c>
+      <c r="H60" s="26"/>
+    </row>
+    <row r="61" spans="2:8" ht="43.8" customHeight="1">
+      <c r="B61" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F61" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G61" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H61" s="26"/>
+    </row>
+    <row r="62" spans="2:8" ht="30.6" customHeight="1">
+      <c r="B62" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G62" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H62" s="18"/>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="23"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="21"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="21"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="35"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="33"/>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2142,19 +2451,19 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="2" width="31.875" customWidth="1"/>
+    <col min="1" max="1" width="3.3984375" customWidth="1"/>
+    <col min="2" max="2" width="31.8984375" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.625" customWidth="1"/>
-    <col min="6" max="6" width="13.375" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="4" max="5" width="15.59765625" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.3984375" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="3.375" customWidth="1"/>
+    <col min="9" max="9" width="3.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1">
@@ -2264,7 +2573,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
@@ -2470,12 +2779,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="3"/>
+    <col min="1" max="1" width="3.3984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="88.3984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.8984375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
Ata 23/05 e Atualização do plano de ação
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c7235aa8075ae8b/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c7235aa8075ae8b/Área de Trabalho/Noctoramento/Documentacao/Documentação do Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42D6CC88-4966-46F4-B7AA-814279061F1A}"/>
+  <xr:revisionPtr revIDLastSave="274" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA7F931D-F9A0-462F-B644-C4D4D0FB6AD7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="109">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -376,10 +376,10 @@
     <t>Em andamento</t>
   </si>
   <si>
-    <t>Andamento</t>
-  </si>
-  <si>
     <t>Versão final, sem mudanças após</t>
+  </si>
+  <si>
+    <t>VM Windows Server</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -755,15 +755,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -871,6 +862,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1199,11 +1194,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K58" sqref="K58"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1220,28 +1215,28 @@
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:16" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -1255,14 +1250,14 @@
       <c r="B3" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="51"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1325,10 +1320,10 @@
       <c r="D7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="33">
         <v>1</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="34">
         <v>45380</v>
       </c>
       <c r="G7" s="19">
@@ -1348,10 +1343,10 @@
       <c r="D8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="33">
         <v>1</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="34">
         <v>45381</v>
       </c>
       <c r="G8" s="19"/>
@@ -1369,10 +1364,10 @@
       <c r="D9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="33">
         <v>0.9</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="34">
         <v>45381</v>
       </c>
       <c r="G9" s="19"/>
@@ -1390,10 +1385,10 @@
       <c r="D10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="33">
         <v>1</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="34">
         <v>45381</v>
       </c>
       <c r="G10" s="19">
@@ -1413,7 +1408,7 @@
       <c r="D11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="33">
         <v>0.15</v>
       </c>
       <c r="F11" s="19">
@@ -1430,13 +1425,13 @@
       <c r="B12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="40" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="36">
+      <c r="E12" s="33">
         <v>0.5</v>
       </c>
       <c r="F12" s="19">
@@ -1457,7 +1452,7 @@
       <c r="D13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="33">
         <v>0.9</v>
       </c>
       <c r="F13" s="19">
@@ -1469,25 +1464,25 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="37" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1512,7 +1507,7 @@
       <c r="D16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="33">
         <v>0.5</v>
       </c>
       <c r="F16" s="19">
@@ -1524,25 +1519,25 @@
       <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" ht="39" customHeight="1">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="42">
         <v>0</v>
       </c>
-      <c r="F17" s="46">
+      <c r="F17" s="43">
         <v>45390</v>
       </c>
-      <c r="G17" s="46">
+      <c r="G17" s="43">
         <v>45396</v>
       </c>
-      <c r="H17" s="44" t="s">
+      <c r="H17" s="41" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1556,7 +1551,7 @@
       <c r="D18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="33">
         <v>0</v>
       </c>
       <c r="F18" s="19">
@@ -1577,7 +1572,7 @@
       <c r="D19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="36">
+      <c r="E19" s="33">
         <v>0</v>
       </c>
       <c r="F19" s="19">
@@ -1598,7 +1593,7 @@
       <c r="D20" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="33">
         <v>0</v>
       </c>
       <c r="F20" s="19">
@@ -1619,7 +1614,7 @@
       <c r="D21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="36">
+      <c r="E21" s="33">
         <v>1</v>
       </c>
       <c r="F21" s="19">
@@ -1640,7 +1635,7 @@
       <c r="D22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="36">
+      <c r="E22" s="33">
         <v>1</v>
       </c>
       <c r="F22" s="19">
@@ -1661,7 +1656,7 @@
       <c r="D23" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="33">
         <v>1</v>
       </c>
       <c r="F23" s="19">
@@ -1680,7 +1675,7 @@
       <c r="D24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="33">
         <v>0</v>
       </c>
       <c r="F24" s="19">
@@ -1701,7 +1696,7 @@
       <c r="D25" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="33">
         <v>1</v>
       </c>
       <c r="F25" s="19">
@@ -1722,7 +1717,7 @@
       <c r="D26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="36">
+      <c r="E26" s="33">
         <v>0.3</v>
       </c>
       <c r="F26" s="19">
@@ -1743,7 +1738,7 @@
       <c r="D27" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="33">
         <v>1</v>
       </c>
       <c r="F27" s="19">
@@ -1762,7 +1757,7 @@
       <c r="D28" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="36">
+      <c r="E28" s="33">
         <v>0</v>
       </c>
       <c r="F28" s="19">
@@ -1779,7 +1774,7 @@
       <c r="D29" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="33">
         <v>0</v>
       </c>
       <c r="F29" s="19">
@@ -1796,7 +1791,7 @@
       <c r="D30" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="36">
+      <c r="E30" s="33">
         <v>0</v>
       </c>
       <c r="F30" s="19">
@@ -1813,7 +1808,7 @@
       <c r="D31" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="36">
+      <c r="E31" s="33">
         <v>0</v>
       </c>
       <c r="F31" s="19">
@@ -1830,7 +1825,7 @@
       <c r="D32" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="33">
         <v>0</v>
       </c>
       <c r="F32" s="19">
@@ -1849,7 +1844,7 @@
       <c r="D33" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="33">
         <v>0</v>
       </c>
       <c r="F33" s="19">
@@ -1861,25 +1856,25 @@
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="2:8" ht="27" customHeight="1">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="41" t="s">
+      <c r="F34" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="41" t="s">
+      <c r="G34" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="40" t="s">
+      <c r="H34" s="37" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1904,7 +1899,7 @@
       <c r="D36" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="36">
+      <c r="E36" s="33">
         <v>0.5</v>
       </c>
       <c r="F36" s="19"/>
@@ -1921,7 +1916,7 @@
       <c r="D37" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="36">
+      <c r="E37" s="33">
         <v>0.75</v>
       </c>
       <c r="F37" s="19"/>
@@ -1938,7 +1933,7 @@
       <c r="D38" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="36">
+      <c r="E38" s="33">
         <v>0.8</v>
       </c>
       <c r="F38" s="19"/>
@@ -1955,7 +1950,7 @@
       <c r="D39" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="36">
+      <c r="E39" s="33">
         <v>0.6</v>
       </c>
       <c r="F39" s="19"/>
@@ -1972,7 +1967,7 @@
       <c r="D40" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="36">
+      <c r="E40" s="33">
         <v>0</v>
       </c>
       <c r="F40" s="19"/>
@@ -1989,7 +1984,7 @@
       <c r="D41" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="36">
+      <c r="E41" s="33">
         <v>0</v>
       </c>
       <c r="F41" s="19"/>
@@ -2097,7 +2092,7 @@
       <c r="D49" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="42" t="s">
+      <c r="E49" s="39" t="s">
         <v>86</v>
       </c>
       <c r="F49" s="32">
@@ -2113,12 +2108,12 @@
         <v>78</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D50" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="42" t="s">
+      <c r="E50" s="39" t="s">
         <v>86</v>
       </c>
       <c r="F50" s="32">
@@ -2139,8 +2134,8 @@
       <c r="D51" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E51" s="36" t="s">
-        <v>86</v>
+      <c r="E51" s="33" t="s">
+        <v>106</v>
       </c>
       <c r="F51" s="19">
         <v>45429</v>
@@ -2186,7 +2181,7 @@
         <v>20</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F53" s="19">
         <v>45429</v>
@@ -2195,7 +2190,7 @@
         <v>45413</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="2:8" ht="34.35" customHeight="1">
@@ -2209,7 +2204,7 @@
         <v>20</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F54" s="19">
         <v>45429</v>
@@ -2251,7 +2246,7 @@
         <v>20</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="F56" s="19">
         <v>45429</v>
@@ -2274,7 +2269,7 @@
         <v>20</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="F57" s="19">
         <v>45429</v>
@@ -2318,7 +2313,7 @@
         <v>20</v>
       </c>
       <c r="E59" s="27" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="F59" s="32">
         <v>45429</v>
@@ -2339,7 +2334,7 @@
         <v>20</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="F60" s="19">
         <v>45429</v>
@@ -2360,7 +2355,7 @@
         <v>20</v>
       </c>
       <c r="E61" s="27" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="F61" s="32">
         <v>45429</v>
@@ -2381,7 +2376,7 @@
         <v>20</v>
       </c>
       <c r="E62" s="27" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="F62" s="32">
         <v>45429</v>
@@ -2412,22 +2407,151 @@
       <c r="H64" s="21"/>
     </row>
     <row r="65" spans="2:8">
-      <c r="B65" s="33"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="33"/>
+      <c r="B65" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="66" spans="2:8">
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
+      <c r="B66" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F66" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G66" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H66" s="26"/>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E67" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F67" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G67" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H67" s="26"/>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F68" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G68" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H68" s="26"/>
+    </row>
+    <row r="69" spans="2:8">
+      <c r="B69" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E69" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F69" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G69" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H69" s="26"/>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F70" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G70" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H70" s="26"/>
+    </row>
+    <row r="71" spans="2:8">
+      <c r="B71" s="26"/>
+      <c r="C71" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E71" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F71" s="32">
+        <v>45429</v>
+      </c>
+      <c r="G71" s="32">
+        <v>45413</v>
+      </c>
+      <c r="H71" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Atualizando plano de ação
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c7235aa8075ae8b/Área de Trabalho/Noctoramento/Documentacao/Documentação do Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="274" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA7F931D-F9A0-462F-B644-C4D4D0FB6AD7}"/>
+  <xr:revisionPtr revIDLastSave="327" documentId="13_ncr:1_{75086E89-9684-435B-9183-886507076373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BFBAF9A-B34F-4FEE-B4B3-475F4E8DD077}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="119">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -379,7 +379,37 @@
     <t>Versão final, sem mudanças após</t>
   </si>
   <si>
-    <t>VM Windows Server</t>
+    <t>29/05 -&gt; 02/06</t>
+  </si>
+  <si>
+    <t>Script instalação</t>
+  </si>
+  <si>
+    <t>Andamento</t>
+  </si>
+  <si>
+    <t>xx/05/2024</t>
+  </si>
+  <si>
+    <t>CRUDS do site</t>
+  </si>
+  <si>
+    <t>Ligação site com banco de dados (web-data-viz)</t>
+  </si>
+  <si>
+    <t>Ligação do cadastro e login ao banco</t>
+  </si>
+  <si>
+    <t>Pedro Sarabando</t>
+  </si>
+  <si>
+    <t>Jar Grupo Completo ligado ao banco de dados</t>
+  </si>
+  <si>
+    <t>Dashs Dinâmicas ligadas ao  banco de dados</t>
+  </si>
+  <si>
+    <t>PPTX</t>
   </si>
 </sst>
 </file>
@@ -862,10 +892,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1194,11 +1220,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -2398,7 +2424,9 @@
       <c r="H63" s="23"/>
     </row>
     <row r="64" spans="2:8">
-      <c r="B64" s="21"/>
+      <c r="B64" s="21" t="s">
+        <v>108</v>
+      </c>
       <c r="C64" s="30"/>
       <c r="D64" s="30"/>
       <c r="E64" s="30"/>
@@ -2431,22 +2459,22 @@
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="26" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D66" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F66" s="32">
-        <v>45429</v>
+        <v>110</v>
+      </c>
+      <c r="F66" s="32" t="s">
+        <v>111</v>
       </c>
       <c r="G66" s="32">
-        <v>45413</v>
+        <v>45445</v>
       </c>
       <c r="H66" s="26"/>
     </row>
@@ -2455,19 +2483,19 @@
         <v>78</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D67" s="27" t="s">
         <v>85</v>
       </c>
       <c r="E67" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F67" s="32">
-        <v>45429</v>
+        <v>110</v>
+      </c>
+      <c r="F67" s="32" t="s">
+        <v>111</v>
       </c>
       <c r="G67" s="32">
-        <v>45413</v>
+        <v>45445</v>
       </c>
       <c r="H67" s="26"/>
     </row>
@@ -2476,82 +2504,128 @@
         <v>97</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D68" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F68" s="32">
-        <v>45429</v>
+        <v>110</v>
+      </c>
+      <c r="F68" s="32" t="s">
+        <v>111</v>
       </c>
       <c r="G68" s="32">
-        <v>45413</v>
+        <v>45445</v>
       </c>
       <c r="H68" s="26"/>
     </row>
     <row r="69" spans="2:8">
       <c r="B69" s="26" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="E69" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F69" s="32">
-        <v>45429</v>
+        <v>110</v>
+      </c>
+      <c r="F69" s="32" t="s">
+        <v>111</v>
       </c>
       <c r="G69" s="32">
-        <v>45413</v>
+        <v>45445</v>
       </c>
       <c r="H69" s="26"/>
     </row>
-    <row r="70" spans="2:8">
+    <row r="70" spans="2:8" ht="26.4">
       <c r="B70" s="26" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="D70" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F70" s="32">
-        <v>45429</v>
+        <v>110</v>
+      </c>
+      <c r="F70" s="32" t="s">
+        <v>111</v>
       </c>
       <c r="G70" s="32">
-        <v>45413</v>
-      </c>
-      <c r="H70" s="26"/>
+        <v>45445</v>
+      </c>
+      <c r="H70" s="26" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="71" spans="2:8">
-      <c r="B71" s="26"/>
+      <c r="B71" s="26" t="s">
+        <v>117</v>
+      </c>
       <c r="C71" s="27" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D71" s="27" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="E71" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F71" s="32">
-        <v>45429</v>
+        <v>110</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>111</v>
       </c>
       <c r="G71" s="32">
-        <v>45413</v>
+        <v>45445</v>
       </c>
       <c r="H71" s="26"/>
+    </row>
+    <row r="72" spans="2:8">
+      <c r="B72" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G72" s="32">
+        <v>45445</v>
+      </c>
+      <c r="H72" s="26"/>
+    </row>
+    <row r="73" spans="2:8">
+      <c r="B73" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C73" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F73" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G73" s="32">
+        <v>45445</v>
+      </c>
+      <c r="H73" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Criando uma pasta com a documentação final da Noctoramento
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/PlanoDeAcao.xlsx
+++ b/Documentação do Projeto/PlanoDeAcao.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -892,6 +892,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>